<commit_message>
added test version of full dataset commands, fixed error in test_ananlysis commands
</commit_message>
<xml_diff>
--- a/datasets/AMETHST_data/amethst_commands.xlsx
+++ b/datasets/AMETHST_data/amethst_commands.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3340" yWindow="0" windowWidth="34120" windowHeight="20360" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="3340" yWindow="0" windowWidth="34120" windowHeight="20360" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="amethst_commands" sheetId="1" r:id="rId1"/>
-    <sheet name="commands pasted as simple text" sheetId="2" r:id="rId2"/>
+    <sheet name="full commands text" sheetId="2" r:id="rId2"/>
+    <sheet name="test commands text" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2735" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3004" uniqueCount="591">
   <si>
     <t>#job</t>
   </si>
@@ -1469,6 +1470,330 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 4.MG-RAST.MG-RAST_default.included.norm --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method bray-curtis --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_1w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 4.MG-RAST.MG-RAST_default.included.norm --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method bray-curtis --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_1b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 3.MG-RAST.MG-RAST_default.included.raw --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method bray-curtis --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_2w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 3.MG-RAST.MG-RAST_default.included.raw --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method bray-curtis --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_2b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 4.MG-RAST.MG-RAST_default.included.norm --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_3w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 4.MG-RAST.MG-RAST_default.included.norm --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_3b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 3.MG-RAST.MG-RAST_default.included.raw --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_4w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 3.MG-RAST.MG-RAST_default.included.raw --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_4b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 11.Qiime.Qiime_default.included.raw --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_5w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 11.Qiime.Qiime_default.included.raw --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_5b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 12.Qiime.Qiime_default.included.norm --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_6w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 12.Qiime.Qiime_default.included.norm --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_6b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 11.Qiime.Qiime_default.included.raw --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_7w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 11.Qiime.Qiime_default.included.raw --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_7b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 2.MG-RAST.MG-RAST_default.removed.norm --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method bray-curtis --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_8w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 2.MG-RAST.MG-RAST_default.removed.norm --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method bray-curtis --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_8b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 1.MG-RAST.MG-RAST_default.removed.raw --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method bray-curtis --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_9w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 1.MG-RAST.MG-RAST_default.removed.raw --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method bray-curtis --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_9b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 2.MG-RAST.MG-RAST_default.removed.norm --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_10w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 2.MG-RAST.MG-RAST_default.removed.norm --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_10b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 1.MG-RAST.MG-RAST_default.removed.raw --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_11w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 1.MG-RAST.MG-RAST_default.removed.raw --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_11b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 9.Qiime.Qiime_default.removed.raw --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_12w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 9.Qiime.Qiime_default.removed.raw --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_12b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 10.Qiime.Qiime_default.removed.norm --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_13w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 10.Qiime.Qiime_default.removed.norm --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_13b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 9.Qiime.Qiime_default.removed.raw --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_14w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 9.Qiime.Qiime_default.removed.raw --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_14b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 8.MG-RAST.100p.included.norm --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method bray-curtis --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_15w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 8.MG-RAST.100p.included.norm --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method bray-curtis --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_15b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 7.MG-RAST.100p.included.raw --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method bray-curtis --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_16w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 7.MG-RAST.100p.included.raw --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method bray-curtis --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_16b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 8.MG-RAST.100p.included.norm --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_17w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 8.MG-RAST.100p.included.norm --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_17b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 7.MG-RAST.100p.included.raw --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_18w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 7.MG-RAST.100p.included.raw --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_18b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_19w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_19b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 16.Qiime.100p.included.norm --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_20w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 16.Qiime.100p.included.norm --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_20b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_21w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_21b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 6.MG-RAST.100p.removed.norm --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method bray-curtis --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_22w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 6.MG-RAST.100p.removed.norm --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method bray-curtis --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_22b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 5.MG-RAST.100p.removed.raw --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method bray-curtis --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_23w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 5.MG-RAST.100p.removed.raw --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method bray-curtis --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_23b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 6.MG-RAST.100p.removed.norm --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_24w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 6.MG-RAST.100p.removed.norm --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_24b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 5.MG-RAST.100p.removed.raw --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_25w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 5.MG-RAST.100p.removed.raw --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_25b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_26w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_26b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 14.Qiime.100p.removed.norm --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_27w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 14.Qiime.100p.removed.norm --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_27b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_28w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_28b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 3.MG-RAST.MG-RAST_default.included.raw --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_29w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 3.MG-RAST.MG-RAST_default.included.raw --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_29b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 4.MG-RAST.MG-RAST_default.included.norm --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_30w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 4.MG-RAST.MG-RAST_default.included.norm --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_30b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 7.MG-RAST.100p.included.raw --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_31w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 7.MG-RAST.100p.included.raw --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_31b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 8.MG-RAST.100p.included.norm --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_32w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 8.MG-RAST.100p.included.norm --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_32b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 3.MG-RAST.MG-RAST_default.included.raw --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_33w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 3.MG-RAST.MG-RAST_default.included.raw --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_33b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 4.MG-RAST.MG-RAST_default.included.norm --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_34w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 4.MG-RAST.MG-RAST_default.included.norm --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_34b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 7.MG-RAST.100p.included.raw --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_35w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 7.MG-RAST.100p.included.raw --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_35b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 8.MG-RAST.100p.included.norm --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_36w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 8.MG-RAST.100p.included.norm --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 Analysis_36b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 3.MG-RAST.MG-RAST_default.included.raw --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method OTU --dist_pipe OTU_pipe --num_cpus 10 Analysis_37w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 3.MG-RAST.MG-RAST_default.included.raw --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method OTU --dist_pipe OTU_pipe --num_cpus 10 Analysis_37b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 3.MG-RAST.MG-RAST_default.included.raw --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method w_OTU --dist_pipe OTU_pipe --num_cpus 10 Analysis_38w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 3.MG-RAST.MG-RAST_default.included.raw --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method w_OTU --dist_pipe OTU_pipe --num_cpus 10 Analysis_38b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_39w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_39b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 16.Qiime.100p.included.norm --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_40w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 16.Qiime.100p.included.norm --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_40b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_41w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_41b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 14.Qiime.100p.removed.norm --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_42w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 14.Qiime.100p.removed.norm --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_42b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_43w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_43b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 16.Qiime.100p.included.norm --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_44w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 16.Qiime.100p.included.norm --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_44b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_45w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_45b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 14.Qiime.100p.removed.norm --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_46w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 14.Qiime.100p.removed.norm --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_46b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 11.Qiime.Qiime_default.included.raw --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_47w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 11.Qiime.Qiime_default.included.raw --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_47b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 11.Qiime.Qiime_default.included.raw --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_48w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 11.Qiime.Qiime_default.included.raw --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_48b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 9.Qiime.Qiime_default.removed.raw --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_49w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 9.Qiime.Qiime_default.removed.raw --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_49b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 9.Qiime.Qiime_default.removed.raw --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_50w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 9.Qiime.Qiime_default.removed.raw --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_50b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 12.Qiime.Qiime_default.included.norm --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_51w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 12.Qiime.Qiime_default.included.norm --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_51b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 12.Qiime.Qiime_default.included.norm --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_52w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 12.Qiime.Qiime_default.included.norm --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_52b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 10.Qiime.Qiime_default.removed.norm --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_53w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 10.Qiime.Qiime_default.removed.norm --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_53b --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 10.Qiime.Qiime_default.removed.norm --groups_list AMETHST.groups --num_perm 10 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_54w --cleanup</t>
+  </si>
+  <si>
+    <t>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 10.Qiime.Qiime_default.removed.norm --groups_list AMETHST.groups --num_perm 10 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_54b --cleanup</t>
   </si>
 </sst>
 </file>
@@ -1517,8 +1842,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1558,7 +1885,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1576,6 +1903,7 @@
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1593,6 +1921,7 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4419,7 +4748,7 @@
     </row>
     <row r="70" spans="1:24">
       <c r="X70" t="str">
-        <f t="shared" ref="X69:X132" si="1">CONCATENATE(A70," ",B70," ",C70," ",D70," ",E70," ",F70," ",G70," ",H70," ",I70," ",J70," ",K70," ",L70," ",M70," ",N70," ",O70," ",P70," ",Q70," ",R70," ",S70," ",T70," ",U70," ",V70)</f>
+        <f t="shared" ref="X70:X130" si="1">CONCATENATE(A70," ",B70," ",C70," ",D70," ",E70," ",F70," ",G70," ",H70," ",I70," ",J70," ",K70," ",L70," ",M70," ",N70," ",O70," ",P70," ",Q70," ",R70," ",S70," ",T70," ",U70," ",V70)</f>
         <v xml:space="preserve">                     </v>
       </c>
     </row>
@@ -6684,7 +7013,7 @@
     </row>
     <row r="135" spans="1:24">
       <c r="X135" t="str">
-        <f t="shared" ref="X133:X196" si="2">CONCATENATE(A135," ",B135," ",C135," ",D135," ",E135," ",F135," ",G135," ",H135," ",I135," ",J135," ",K135," ",L135," ",M135," ",N135," ",O135," ",P135," ",Q135," ",R135," ",S135," ",T135," ",U135," ",V135)</f>
+        <f t="shared" ref="X135:X195" si="2">CONCATENATE(A135," ",B135," ",C135," ",D135," ",E135," ",F135," ",G135," ",H135," ",I135," ",J135," ",K135," ",L135," ",M135," ",N135," ",O135," ",P135," ",Q135," ",R135," ",S135," ",T135," ",U135," ",V135)</f>
         <v xml:space="preserve">                     </v>
       </c>
     </row>
@@ -8901,7 +9230,7 @@
     </row>
     <row r="200" spans="1:24">
       <c r="X200" t="str">
-        <f t="shared" ref="X197:X260" si="3">CONCATENATE(A200," ",B200," ",C200," ",D200," ",E200," ",F200," ",G200," ",H200," ",I200," ",J200," ",K200," ",L200," ",M200," ",N200," ",O200," ",P200," ",Q200," ",R200," ",S200," ",T200," ",U200," ",V200)</f>
+        <f t="shared" ref="X200:X260" si="3">CONCATENATE(A200," ",B200," ",C200," ",D200," ",E200," ",F200," ",G200," ",H200," ",I200," ",J200," ",K200," ",L200," ",M200," ",N200," ",O200," ",P200," ",Q200," ",R200," ",S200," ",T200," ",U200," ",V200)</f>
         <v xml:space="preserve">                     </v>
       </c>
     </row>
@@ -11289,7 +11618,7 @@
         <v>265</v>
       </c>
       <c r="X262" t="str">
-        <f t="shared" ref="X261:X269" si="4">CONCATENATE(A262," ",B262," ",C262," ",D262," ",E262," ",F262," ",G262," ",H262," ",I262," ",J262," ",K262," ",L262," ",M262," ",N262," ",O262," ",P262," ",Q262," ",R262," ",S262," ",T262," ",U262," ",V262)</f>
+        <f t="shared" ref="X262:X268" si="4">CONCATENATE(A262," ",B262," ",C262," ",D262," ",E262," ",F262," ",G262," ",H262," ",I262," ",J262," ",K262," ",L262," ",M262," ",N262," ",O262," ",P262," ",Q262," ",R262," ",S262," ",T262," ",U262," ",V262)</f>
         <v>~/AMETHST/plot_pco_with_stats_all.3-4-13.pl --data_file 10.Qiime.Qiime_default.removed.norm --groups_list AMETHST.groups --num_perm 1000 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_53w --cleanup</v>
       </c>
     </row>
@@ -11608,8 +11937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A269"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G51" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -12968,4 +13297,1369 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A269"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A215" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1">
+      <c r="A120" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1">
+      <c r="A122" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1">
+      <c r="A123" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1">
+      <c r="A124" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1">
+      <c r="A125" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1">
+      <c r="A126" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1">
+      <c r="A127" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1">
+      <c r="A128" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1">
+      <c r="A129" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1">
+      <c r="A130" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1">
+      <c r="A132" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1">
+      <c r="A133" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1">
+      <c r="A134" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1">
+      <c r="A135" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1">
+      <c r="A136" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1">
+      <c r="A137" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1">
+      <c r="A138" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1">
+      <c r="A139" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1">
+      <c r="A140" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1">
+      <c r="A141" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1">
+      <c r="A142" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1">
+      <c r="A143" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1">
+      <c r="A144" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1">
+      <c r="A145" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1">
+      <c r="A146" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1">
+      <c r="A147" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1">
+      <c r="A148" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1">
+      <c r="A149" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1">
+      <c r="A150" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1">
+      <c r="A151" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1">
+      <c r="A152" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1">
+      <c r="A153" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1">
+      <c r="A154" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1">
+      <c r="A155" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1">
+      <c r="A156" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1">
+      <c r="A157" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1">
+      <c r="A158" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1">
+      <c r="A159" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1">
+      <c r="A160" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1">
+      <c r="A161" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1">
+      <c r="A162" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1">
+      <c r="A163" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1">
+      <c r="A164" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1">
+      <c r="A165" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1">
+      <c r="A166" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1">
+      <c r="A167" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1">
+      <c r="A168" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1">
+      <c r="A169" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1">
+      <c r="A170" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1">
+      <c r="A171" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1">
+      <c r="A172" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1">
+      <c r="A173" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1">
+      <c r="A174" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1">
+      <c r="A175" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1">
+      <c r="A176" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1">
+      <c r="A177" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1">
+      <c r="A178" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1">
+      <c r="A179" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1">
+      <c r="A180" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1">
+      <c r="A181" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1">
+      <c r="A182" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1">
+      <c r="A183" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1">
+      <c r="A184" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1">
+      <c r="A185" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1">
+      <c r="A186" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1">
+      <c r="A187" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1">
+      <c r="A188" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1">
+      <c r="A189" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1">
+      <c r="A190" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1">
+      <c r="A191" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1">
+      <c r="A192" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1">
+      <c r="A193" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1">
+      <c r="A194" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1">
+      <c r="A195" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1">
+      <c r="A196" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1">
+      <c r="A197" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1">
+      <c r="A198" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1">
+      <c r="A199" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1">
+      <c r="A200" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1">
+      <c r="A201" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1">
+      <c r="A202" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1">
+      <c r="A203" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1">
+      <c r="A204" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1">
+      <c r="A205" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1">
+      <c r="A206" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1">
+      <c r="A207" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1">
+      <c r="A208" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1">
+      <c r="A209" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1">
+      <c r="A210" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1">
+      <c r="A211" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1">
+      <c r="A212" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1">
+      <c r="A213" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1">
+      <c r="A214" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1">
+      <c r="A215" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1">
+      <c r="A216" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1">
+      <c r="A217" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1">
+      <c r="A218" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1">
+      <c r="A219" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1">
+      <c r="A220" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1">
+      <c r="A221" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1">
+      <c r="A222" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1">
+      <c r="A223" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1">
+      <c r="A224" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1">
+      <c r="A225" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1">
+      <c r="A226" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1">
+      <c r="A227" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1">
+      <c r="A228" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1">
+      <c r="A229" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1">
+      <c r="A230" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1">
+      <c r="A231" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1">
+      <c r="A232" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1">
+      <c r="A233" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1">
+      <c r="A234" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1">
+      <c r="A235" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1">
+      <c r="A236" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1">
+      <c r="A237" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1">
+      <c r="A238" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1">
+      <c r="A239" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1">
+      <c r="A240" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1">
+      <c r="A241" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1">
+      <c r="A242" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1">
+      <c r="A243" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1">
+      <c r="A244" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1">
+      <c r="A245" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1">
+      <c r="A246" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1">
+      <c r="A247" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1">
+      <c r="A248" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1">
+      <c r="A249" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1">
+      <c r="A250" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1">
+      <c r="A251" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1">
+      <c r="A252" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1">
+      <c r="A253" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1">
+      <c r="A254" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1">
+      <c r="A255" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1">
+      <c r="A256" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1">
+      <c r="A257" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1">
+      <c r="A258" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1">
+      <c r="A259" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1">
+      <c r="A260" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1">
+      <c r="A261" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1">
+      <c r="A262" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1">
+      <c r="A263" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1">
+      <c r="A264" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1">
+      <c r="A265" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1">
+      <c r="A266" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1">
+      <c r="A267" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1">
+      <c r="A268" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1">
+      <c r="A269" t="s">
+        <v>481</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
edits to commands file, slight change to main log
</commit_message>
<xml_diff>
--- a/datasets/AMETHST_data/amethst_commands.xlsx
+++ b/datasets/AMETHST_data/amethst_commands.xlsx
@@ -917,30 +917,12 @@
     <t>combine_summary_stats.pl --file_search_mode pattern --within_pattern Analysis_18w --between_pattern Analysis_18b --groups_list AMETHST.PCoA.groups</t>
   </si>
   <si>
-    <t>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_19w --cleanup</t>
-  </si>
-  <si>
-    <t>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_19b --cleanup</t>
-  </si>
-  <si>
     <t>combine_summary_stats.pl --file_search_mode pattern --within_pattern Analysis_19w --between_pattern Analysis_19b --groups_list AMETHST.PCoA.groups</t>
   </si>
   <si>
-    <t>plot_pco_with_stats_all.pl --data_file 16.Qiime.100p.included.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_20w --cleanup</t>
-  </si>
-  <si>
-    <t>plot_pco_with_stats_all.pl --data_file 16.Qiime.100p.included.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_20b --cleanup</t>
-  </si>
-  <si>
     <t>combine_summary_stats.pl --file_search_mode pattern --within_pattern Analysis_20w --between_pattern Analysis_20b --groups_list AMETHST.PCoA.groups</t>
   </si>
   <si>
-    <t>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_21w --cleanup</t>
-  </si>
-  <si>
-    <t>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_21b --cleanup</t>
-  </si>
-  <si>
     <t>combine_summary_stats.pl --file_search_mode pattern --within_pattern Analysis_21w --between_pattern Analysis_21b --groups_list AMETHST.PCoA.groups</t>
   </si>
   <si>
@@ -956,30 +938,12 @@
     <t>combine_summary_stats.pl --file_search_mode pattern --within_pattern Analysis_25w --between_pattern Analysis_25b --groups_list AMETHST.PCoA.groups</t>
   </si>
   <si>
-    <t>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_26w --cleanup</t>
-  </si>
-  <si>
-    <t>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_26b --cleanup</t>
-  </si>
-  <si>
     <t>combine_summary_stats.pl --file_search_mode pattern --within_pattern Analysis_26w --between_pattern Analysis_26b --groups_list AMETHST.PCoA.groups</t>
   </si>
   <si>
-    <t>plot_pco_with_stats_all.pl --data_file 14.Qiime.100p.removed.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_27w --cleanup</t>
-  </si>
-  <si>
-    <t>plot_pco_with_stats_all.pl --data_file 14.Qiime.100p.removed.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_27b --cleanup</t>
-  </si>
-  <si>
     <t>combine_summary_stats.pl --file_search_mode pattern --within_pattern Analysis_27w --between_pattern Analysis_27b --groups_list AMETHST.PCoA.groups</t>
   </si>
   <si>
-    <t>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_28w --cleanup</t>
-  </si>
-  <si>
-    <t>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_28b --cleanup</t>
-  </si>
-  <si>
     <t>combine_summary_stats.pl --file_search_mode pattern --within_pattern Analysis_28w --between_pattern Analysis_28b --groups_list AMETHST.PCoA.groups</t>
   </si>
   <si>
@@ -1013,75 +977,27 @@
     <t>combine_summary_stats.pl --file_search_mode pattern --within_pattern Analysis_38w --between_pattern Analysis_38b --groups_list AMETHST.PCoA.groups</t>
   </si>
   <si>
-    <t>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_39w --cleanup</t>
-  </si>
-  <si>
-    <t>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_39b --cleanup</t>
-  </si>
-  <si>
     <t>combine_summary_stats.pl --file_search_mode pattern --within_pattern Analysis_39w --between_pattern Analysis_39b --groups_list AMETHST.PCoA.groups</t>
   </si>
   <si>
-    <t>plot_pco_with_stats_all.pl --data_file 16.Qiime.100p.included.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_40w --cleanup</t>
-  </si>
-  <si>
-    <t>plot_pco_with_stats_all.pl --data_file 16.Qiime.100p.included.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_40b --cleanup</t>
-  </si>
-  <si>
     <t>combine_summary_stats.pl --file_search_mode pattern --within_pattern Analysis_40w --between_pattern Analysis_40b --groups_list AMETHST.PCoA.groups</t>
   </si>
   <si>
-    <t>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_41w --cleanup</t>
-  </si>
-  <si>
-    <t>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_41b --cleanup</t>
-  </si>
-  <si>
     <t>combine_summary_stats.pl --file_search_mode pattern --within_pattern Analysis_41w --between_pattern Analysis_41b --groups_list AMETHST.PCoA.groups</t>
   </si>
   <si>
-    <t>plot_pco_with_stats_all.pl --data_file 14.Qiime.100p.removed.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_42w --cleanup</t>
-  </si>
-  <si>
-    <t>plot_pco_with_stats_all.pl --data_file 14.Qiime.100p.removed.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_42b --cleanup</t>
-  </si>
-  <si>
     <t>combine_summary_stats.pl --file_search_mode pattern --within_pattern Analysis_42w --between_pattern Analysis_42b --groups_list AMETHST.PCoA.groups</t>
   </si>
   <si>
-    <t>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_43w --cleanup</t>
-  </si>
-  <si>
-    <t>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_43b --cleanup</t>
-  </si>
-  <si>
     <t>combine_summary_stats.pl --file_search_mode pattern --within_pattern Analysis_43w --between_pattern Analysis_43b --groups_list AMETHST.PCoA.groups</t>
   </si>
   <si>
-    <t>plot_pco_with_stats_all.pl --data_file 16.Qiime.100p.included.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_44w --cleanup</t>
-  </si>
-  <si>
-    <t>plot_pco_with_stats_all.pl --data_file 16.Qiime.100p.included.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_44b --cleanup</t>
-  </si>
-  <si>
     <t>combine_summary_stats.pl --file_search_mode pattern --within_pattern Analysis_44w --between_pattern Analysis_44b --groups_list AMETHST.PCoA.groups</t>
   </si>
   <si>
-    <t>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_45w --cleanup</t>
-  </si>
-  <si>
-    <t>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_45b --cleanup</t>
-  </si>
-  <si>
     <t>combine_summary_stats.pl --file_search_mode pattern --within_pattern Analysis_45w --between_pattern Analysis_45b --groups_list AMETHST.PCoA.groups</t>
   </si>
   <si>
-    <t>plot_pco_with_stats_all.pl --data_file 14.Qiime.100p.removed.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_46w --cleanup</t>
-  </si>
-  <si>
-    <t>plot_pco_with_stats_all.pl --data_file 14.Qiime.100p.removed.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_46b --cleanup</t>
-  </si>
-  <si>
     <t>combine_summary_stats.pl --file_search_mode pattern --within_pattern Analysis_46w --between_pattern Analysis_46b --groups_list AMETHST.PCoA.groups</t>
   </si>
   <si>
@@ -1193,90 +1109,6 @@
     <t>plot_pco_with_stats_all.pl --data_file 9.Qiime.Qiime_default.removed.raw --groups_list AMETHST.stat.groups --num_perm 10 --perm_type rowwise_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_14b --cleanup</t>
   </si>
   <si>
-    <t>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 10 --perm_type dataset_rand --dist_method unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_19w --cleanup</t>
-  </si>
-  <si>
-    <t>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 10 --perm_type rowwise_rand --dist_method unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_19b --cleanup</t>
-  </si>
-  <si>
-    <t>plot_pco_with_stats_all.pl --data_file 16.Qiime.100p.included.norm --groups_list AMETHST.stat.groups --num_perm 10 --perm_type dataset_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_20w --cleanup</t>
-  </si>
-  <si>
-    <t>plot_pco_with_stats_all.pl --data_file 16.Qiime.100p.included.norm --groups_list AMETHST.stat.groups --num_perm 10 --perm_type rowwise_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_20b --cleanup</t>
-  </si>
-  <si>
-    <t>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 10 --perm_type dataset_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_21w --cleanup</t>
-  </si>
-  <si>
-    <t>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 10 --perm_type rowwise_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_21b --cleanup</t>
-  </si>
-  <si>
-    <t>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 10 --perm_type dataset_rand --dist_method unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_26w --cleanup</t>
-  </si>
-  <si>
-    <t>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 10 --perm_type rowwise_rand --dist_method unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_26b --cleanup</t>
-  </si>
-  <si>
-    <t>plot_pco_with_stats_all.pl --data_file 14.Qiime.100p.removed.norm --groups_list AMETHST.stat.groups --num_perm 10 --perm_type dataset_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_27w --cleanup</t>
-  </si>
-  <si>
-    <t>plot_pco_with_stats_all.pl --data_file 14.Qiime.100p.removed.norm --groups_list AMETHST.stat.groups --num_perm 10 --perm_type rowwise_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_27b --cleanup</t>
-  </si>
-  <si>
-    <t>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 10 --perm_type dataset_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_28w --cleanup</t>
-  </si>
-  <si>
-    <t>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 10 --perm_type rowwise_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_28b --cleanup</t>
-  </si>
-  <si>
-    <t>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 10 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_39w --cleanup</t>
-  </si>
-  <si>
-    <t>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 10 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_39b --cleanup</t>
-  </si>
-  <si>
-    <t>plot_pco_with_stats_all.pl --data_file 16.Qiime.100p.included.norm --groups_list AMETHST.stat.groups --num_perm 10 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_40w --cleanup</t>
-  </si>
-  <si>
-    <t>plot_pco_with_stats_all.pl --data_file 16.Qiime.100p.included.norm --groups_list AMETHST.stat.groups --num_perm 10 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_40b --cleanup</t>
-  </si>
-  <si>
-    <t>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 10 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_41w --cleanup</t>
-  </si>
-  <si>
-    <t>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 10 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_41b --cleanup</t>
-  </si>
-  <si>
-    <t>plot_pco_with_stats_all.pl --data_file 14.Qiime.100p.removed.norm --groups_list AMETHST.stat.groups --num_perm 10 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_42w --cleanup</t>
-  </si>
-  <si>
-    <t>plot_pco_with_stats_all.pl --data_file 14.Qiime.100p.removed.norm --groups_list AMETHST.stat.groups --num_perm 10 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_42b --cleanup</t>
-  </si>
-  <si>
-    <t>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 10 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_43w --cleanup</t>
-  </si>
-  <si>
-    <t>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 10 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_43b --cleanup</t>
-  </si>
-  <si>
-    <t>plot_pco_with_stats_all.pl --data_file 16.Qiime.100p.included.norm --groups_list AMETHST.stat.groups --num_perm 10 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_44w --cleanup</t>
-  </si>
-  <si>
-    <t>plot_pco_with_stats_all.pl --data_file 16.Qiime.100p.included.norm --groups_list AMETHST.stat.groups --num_perm 10 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_44b --cleanup</t>
-  </si>
-  <si>
-    <t>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 10 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_45w --cleanup</t>
-  </si>
-  <si>
-    <t>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 10 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_45b --cleanup</t>
-  </si>
-  <si>
-    <t>plot_pco_with_stats_all.pl --data_file 14.Qiime.100p.removed.norm --groups_list AMETHST.stat.groups --num_perm 10 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_46w --cleanup</t>
-  </si>
-  <si>
-    <t>plot_pco_with_stats_all.pl --data_file 14.Qiime.100p.removed.norm --groups_list AMETHST.stat.groups --num_perm 10 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_46b --cleanup</t>
-  </si>
-  <si>
     <t>plot_pco_with_stats_all.pl --data_file 11.Qiime.Qiime_default.included.raw --groups_list AMETHST.stat.groups --num_perm 10 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_47w --cleanup</t>
   </si>
   <si>
@@ -1635,6 +1467,174 @@
   </si>
   <si>
     <t>plot_pco_with_stats_all.pl --data_file 3.MG-RAST.MG-RAST_default.included.raw --groups_list AMETHST.stat.groups --num_perm 10 --perm_type rowwise_rand --dist_method w_OTU --dist_pipe OTU_pipe --num_cpus 10 --output_prefix Analysis_38b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_19b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_26w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_19w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 16.Qiime.100p.included.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_20w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 16.Qiime.100p.included.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_20b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_21w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_21b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_26b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 14.Qiime.100p.removed.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_27w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 14.Qiime.100p.removed.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_27b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_28w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_28b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_39w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_39b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 16.Qiime.100p.included.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_40w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 16.Qiime.100p.included.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_40b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_41w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_41b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 14.Qiime.100p.removed.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_42w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 14.Qiime.100p.removed.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_42b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_43w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_43b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 16.Qiime.100p.included.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_44w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 16.Qiime.100p.included.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_44b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_45w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_45b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 14.Qiime.100p.removed.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_46w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 14.Qiime.100p.removed.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_46b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 10 --perm_type dataset_rand --dist_method unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_19w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 10 --perm_type rowwise_rand --dist_method unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_19b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 16.Qiime.100p.included.norm --groups_list AMETHST.stat.groups --num_perm 10 --perm_type dataset_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_20w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 16.Qiime.100p.included.norm --groups_list AMETHST.stat.groups --num_perm 10 --perm_type rowwise_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_20b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 10 --perm_type dataset_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_21w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 10 --perm_type rowwise_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_21b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 10 --perm_type dataset_rand --dist_method unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_26w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 10 --perm_type rowwise_rand --dist_method unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_26b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 14.Qiime.100p.removed.norm --groups_list AMETHST.stat.groups --num_perm 10 --perm_type dataset_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_27w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 14.Qiime.100p.removed.norm --groups_list AMETHST.stat.groups --num_perm 10 --perm_type rowwise_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_27b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 10 --perm_type dataset_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_28w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 10 --perm_type rowwise_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_28b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 10 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_39w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 10 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_39b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 16.Qiime.100p.included.norm --groups_list AMETHST.stat.groups --num_perm 10 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_40w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 16.Qiime.100p.included.norm --groups_list AMETHST.stat.groups --num_perm 10 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_40b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 10 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_41w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 10 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_41b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 14.Qiime.100p.removed.norm --groups_list AMETHST.stat.groups --num_perm 10 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_42w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 14.Qiime.100p.removed.norm --groups_list AMETHST.stat.groups --num_perm 10 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_42b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 10 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_43w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 10 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_43b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 16.Qiime.100p.included.norm --groups_list AMETHST.stat.groups --num_perm 10 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_44w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 16.Qiime.100p.included.norm --groups_list AMETHST.stat.groups --num_perm 10 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_44b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 10 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_45w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 10 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_45b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 14.Qiime.100p.removed.norm --groups_list AMETHST.stat.groups --num_perm 10 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_46w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 14.Qiime.100p.removed.norm --groups_list AMETHST.stat.groups --num_perm 10 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_46b --cleanup</t>
   </si>
 </sst>
 </file>
@@ -1683,8 +1683,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="83">
+  <cellStyleXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1772,7 +1784,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="83">
+  <cellStyles count="95">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1814,6 +1826,12 @@
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1855,6 +1873,12 @@
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2186,7 +2210,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X269"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
+    <sheetView topLeftCell="S1" workbookViewId="0">
       <selection activeCell="X1" sqref="X1:X1048576"/>
     </sheetView>
   </sheetViews>
@@ -4711,7 +4735,7 @@
     </row>
     <row r="70" spans="1:24">
       <c r="X70" t="str">
-        <f t="shared" ref="X70:X130" si="1">CONCATENATE(A70," ",B70," ",C70," ",D70," ",E70," ",F70," ",G70," ",H70," ",I70," ",J70," ",K70," ",L70," ",M70," ",N70," ",O70," ",P70," ",Q70," ",R70," ",S70," ",T70," ",U70," ",V70)</f>
+        <f t="shared" ref="X70:X125" si="1">CONCATENATE(A70," ",B70," ",C70," ",D70," ",E70," ",F70," ",G70," ",H70," ",I70," ",J70," ",K70," ",L70," ",M70," ",N70," ",O70," ",P70," ",Q70," ",R70," ",S70," ",T70," ",U70," ",V70)</f>
         <v xml:space="preserve">                     </v>
       </c>
     </row>
@@ -5461,8 +5485,8 @@
         <v>208</v>
       </c>
       <c r="X92" t="str">
-        <f>CONCATENATE(A92," ",B92," ",C92," ",D92," ",E92," ",F92," ",G92," ",H92," ",I92," ",J92," ",K92," ",L92," ",M92," ",N92," ",O92," ",P92," ",Q92," ",R92," ",S92," ",U92," ",V92)</f>
-        <v>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_19w --cleanup</v>
+        <f>CONCATENATE(A92," ",B92," ",C92," ",D92," ",E92," ",F92," ",G92," ",H92," ",I92," ",J92," ",K92," ",L92," ",M92," ",N92," ",O92," ",P92," ",Q92," ",R92," ",S92," ",T92," ",U92," ",V92)</f>
+        <v>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_19w --cleanup</v>
       </c>
     </row>
     <row r="93" spans="1:24">
@@ -5533,8 +5557,8 @@
         <v>208</v>
       </c>
       <c r="X93" t="str">
-        <f>CONCATENATE(A93," ",B93," ",C93," ",D93," ",E93," ",F93," ",G93," ",H93," ",I93," ",J93," ",K93," ",L93," ",M93," ",N93," ",O93," ",P93," ",Q93," ",R93," ",S93," ",U93," ",V93)</f>
-        <v>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_19b --cleanup</v>
+        <f>CONCATENATE(A93," ",B93," ",C93," ",D93," ",E93," ",F93," ",G93," ",H93," ",I93," ",J93," ",K93," ",L93," ",M93," ",N93," ",O93," ",P93," ",Q93," ",R93," ",S93," ",T93," ",U93," ",V93)</f>
+        <v>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_19b --cleanup</v>
       </c>
     </row>
     <row r="94" spans="1:24">
@@ -5650,8 +5674,8 @@
         <v>208</v>
       </c>
       <c r="X97" t="str">
-        <f>CONCATENATE(A97," ",B97," ",C97," ",D97," ",E97," ",F97," ",G97," ",H97," ",I97," ",J97," ",K97," ",L97," ",M97," ",N97," ",O97," ",P97," ",Q97," ",R97," ",S97," ",U97," ",V97)</f>
-        <v>plot_pco_with_stats_all.pl --data_file 16.Qiime.100p.included.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_20w --cleanup</v>
+        <f>CONCATENATE(A97," ",B97," ",C97," ",D97," ",E97," ",F97," ",G97," ",H97," ",I97," ",J97," ",K97," ",L97," ",M97," ",N97," ",O97," ",P97," ",Q97," ",R97," ",S97," ",T97," ",U97," ",V97)</f>
+        <v>plot_pco_with_stats_all.pl --data_file 16.Qiime.100p.included.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_20w --cleanup</v>
       </c>
     </row>
     <row r="98" spans="1:24">
@@ -5722,8 +5746,8 @@
         <v>208</v>
       </c>
       <c r="X98" t="str">
-        <f>CONCATENATE(A98," ",B98," ",C98," ",D98," ",E98," ",F98," ",G98," ",H98," ",I98," ",J98," ",K98," ",L98," ",M98," ",N98," ",O98," ",P98," ",Q98," ",R98," ",S98," ",U98," ",V98)</f>
-        <v>plot_pco_with_stats_all.pl --data_file 16.Qiime.100p.included.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_20b --cleanup</v>
+        <f>CONCATENATE(A98," ",B98," ",C98," ",D98," ",E98," ",F98," ",G98," ",H98," ",I98," ",J98," ",K98," ",L98," ",M98," ",N98," ",O98," ",P98," ",Q98," ",R98," ",S98," ",T98," ",U98," ",V98)</f>
+        <v>plot_pco_with_stats_all.pl --data_file 16.Qiime.100p.included.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_20b --cleanup</v>
       </c>
     </row>
     <row r="99" spans="1:24">
@@ -5839,8 +5863,8 @@
         <v>208</v>
       </c>
       <c r="X102" t="str">
-        <f>CONCATENATE(A102," ",B102," ",C102," ",D102," ",E102," ",F102," ",G102," ",H102," ",I102," ",J102," ",K102," ",L102," ",M102," ",N102," ",O102," ",P102," ",Q102," ",R102," ",S102," ",U102," ",V102)</f>
-        <v>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_21w --cleanup</v>
+        <f>CONCATENATE(A102," ",B102," ",C102," ",D102," ",E102," ",F102," ",G102," ",H102," ",I102," ",J102," ",K102," ",L102," ",M102," ",N102," ",O102," ",P102," ",Q102," ",R102," ",S102," ",T102," ",U102," ",V102)</f>
+        <v>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_21w --cleanup</v>
       </c>
     </row>
     <row r="103" spans="1:24">
@@ -5911,8 +5935,8 @@
         <v>208</v>
       </c>
       <c r="X103" t="str">
-        <f>CONCATENATE(A103," ",B103," ",C103," ",D103," ",E103," ",F103," ",G103," ",H103," ",I103," ",J103," ",K103," ",L103," ",M103," ",N103," ",O103," ",P103," ",Q103," ",R103," ",S103," ",U103," ",V103)</f>
-        <v>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_21b --cleanup</v>
+        <f>CONCATENATE(A103," ",B103," ",C103," ",D103," ",E103," ",F103," ",G103," ",H103," ",I103," ",J103," ",K103," ",L103," ",M103," ",N103," ",O103," ",P103," ",Q103," ",R103," ",S103," ",T103," ",U103," ",V103)</f>
+        <v>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_21b --cleanup</v>
       </c>
     </row>
     <row r="104" spans="1:24">
@@ -6700,8 +6724,8 @@
         <v>208</v>
       </c>
       <c r="X127" t="str">
-        <f>CONCATENATE(A127," ",B127," ",C127," ",D127," ",E127," ",F127," ",G127," ",H127," ",I127," ",J127," ",K127," ",L127," ",M127," ",N127," ",O127," ",P127," ",Q127," ",R127," ",S127," ",U127," ",V127)</f>
-        <v>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_26w --cleanup</v>
+        <f>CONCATENATE(A127," ",B127," ",C127," ",D127," ",E127," ",F127," ",G127," ",H127," ",I127," ",J127," ",K127," ",L127," ",M127," ",N127," ",O127," ",P127," ",Q127," ",R127," ",S127," ",T127," ",U127," ",V127)</f>
+        <v>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_26w --cleanup</v>
       </c>
     </row>
     <row r="128" spans="1:24">
@@ -6772,8 +6796,8 @@
         <v>208</v>
       </c>
       <c r="X128" t="str">
-        <f>CONCATENATE(A128," ",B128," ",C128," ",D128," ",E128," ",F128," ",G128," ",H128," ",I128," ",J128," ",K128," ",L128," ",M128," ",N128," ",O128," ",P128," ",Q128," ",R128," ",S128," ",U128," ",V128)</f>
-        <v>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_26b --cleanup</v>
+        <f>CONCATENATE(A128," ",B128," ",C128," ",D128," ",E128," ",F128," ",G128," ",H128," ",I128," ",J128," ",K128," ",L128," ",M128," ",N128," ",O128," ",P128," ",Q128," ",R128," ",S128," ",T128," ",U128," ",V128)</f>
+        <v>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_26b --cleanup</v>
       </c>
     </row>
     <row r="129" spans="1:24">
@@ -6889,8 +6913,8 @@
         <v>208</v>
       </c>
       <c r="X132" t="str">
-        <f>CONCATENATE(A132," ",B132," ",C132," ",D132," ",E132," ",F132," ",G132," ",H132," ",I132," ",J132," ",K132," ",L132," ",M132," ",N132," ",O132," ",P132," ",Q132," ",R132," ",S132," ",U132," ",V132)</f>
-        <v>plot_pco_with_stats_all.pl --data_file 14.Qiime.100p.removed.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_27w --cleanup</v>
+        <f>CONCATENATE(A132," ",B132," ",C132," ",D132," ",E132," ",F132," ",G132," ",H132," ",I132," ",J132," ",K132," ",L132," ",M132," ",N132," ",O132," ",P132," ",Q132," ",R132," ",S132," ",T132," ",U132," ",V132)</f>
+        <v>plot_pco_with_stats_all.pl --data_file 14.Qiime.100p.removed.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_27w --cleanup</v>
       </c>
     </row>
     <row r="133" spans="1:24">
@@ -6961,8 +6985,8 @@
         <v>208</v>
       </c>
       <c r="X133" t="str">
-        <f>CONCATENATE(A133," ",B133," ",C133," ",D133," ",E133," ",F133," ",G133," ",H133," ",I133," ",J133," ",K133," ",L133," ",M133," ",N133," ",O133," ",P133," ",Q133," ",R133," ",S133," ",U133," ",V133)</f>
-        <v>plot_pco_with_stats_all.pl --data_file 14.Qiime.100p.removed.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_27b --cleanup</v>
+        <f>CONCATENATE(A133," ",B133," ",C133," ",D133," ",E133," ",F133," ",G133," ",H133," ",I133," ",J133," ",K133," ",L133," ",M133," ",N133," ",O133," ",P133," ",Q133," ",R133," ",S133," ",T133," ",U133," ",V133)</f>
+        <v>plot_pco_with_stats_all.pl --data_file 14.Qiime.100p.removed.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_27b --cleanup</v>
       </c>
     </row>
     <row r="134" spans="1:24">
@@ -7078,8 +7102,8 @@
         <v>208</v>
       </c>
       <c r="X137" t="str">
-        <f>CONCATENATE(A137," ",B137," ",C137," ",D137," ",E137," ",F137," ",G137," ",H137," ",I137," ",J137," ",K137," ",L137," ",M137," ",N137," ",O137," ",P137," ",Q137," ",R137," ",S137," ",U137," ",V137)</f>
-        <v>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_28w --cleanup</v>
+        <f>CONCATENATE(A137," ",B137," ",C137," ",D137," ",E137," ",F137," ",G137," ",H137," ",I137," ",J137," ",K137," ",L137," ",M137," ",N137," ",O137," ",P137," ",Q137," ",R137," ",S137," ",T137," ",U137," ",V137)</f>
+        <v>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_28w --cleanup</v>
       </c>
     </row>
     <row r="138" spans="1:24">
@@ -7150,8 +7174,8 @@
         <v>208</v>
       </c>
       <c r="X138" t="str">
-        <f>CONCATENATE(A138," ",B138," ",C138," ",D138," ",E138," ",F138," ",G138," ",H138," ",I138," ",J138," ",K138," ",L138," ",M138," ",N138," ",O138," ",P138," ",Q138," ",R138," ",S138," ",U138," ",V138)</f>
-        <v>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_28b --cleanup</v>
+        <f>CONCATENATE(A138," ",B138," ",C138," ",D138," ",E138," ",F138," ",G138," ",H138," ",I138," ",J138," ",K138," ",L138," ",M138," ",N138," ",O138," ",P138," ",Q138," ",R138," ",S138," ",T138," ",U138," ",V138)</f>
+        <v>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_28b --cleanup</v>
       </c>
     </row>
     <row r="139" spans="1:24">
@@ -7189,7 +7213,7 @@
     </row>
     <row r="140" spans="1:24">
       <c r="X140" t="str">
-        <f t="shared" ref="X135:X195" si="2">CONCATENATE(A140," ",B140," ",C140," ",D140," ",E140," ",F140," ",G140," ",H140," ",I140," ",J140," ",K140," ",L140," ",M140," ",N140," ",O140," ",P140," ",Q140," ",R140," ",S140," ",T140," ",U140," ",V140)</f>
+        <f t="shared" ref="X140:X190" si="2">CONCATENATE(A140," ",B140," ",C140," ",D140," ",E140," ",F140," ",G140," ",H140," ",I140," ",J140," ",K140," ",L140," ",M140," ",N140," ",O140," ",P140," ",Q140," ",R140," ",S140," ",T140," ",U140," ",V140)</f>
         <v xml:space="preserve">                     </v>
       </c>
     </row>
@@ -8929,8 +8953,8 @@
         <v>208</v>
       </c>
       <c r="X192" t="str">
-        <f>CONCATENATE(A192," ",B192," ",C192," ",D192," ",E192," ",F192," ",G192," ",H192," ",I192," ",J192," ",K192," ",L192," ",M192," ",N192," ",O192," ",P192," ",Q192," ",R192," ",S192," ",U192," ",V192)</f>
-        <v>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_39w --cleanup</v>
+        <f>CONCATENATE(A192," ",B192," ",C192," ",D192," ",E192," ",F192," ",G192," ",H192," ",I192," ",J192," ",K192," ",L192," ",M192," ",N192," ",O192," ",P192," ",Q192," ",R192," ",S192," ",T192," ",U192," ",V192)</f>
+        <v>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_39w --cleanup</v>
       </c>
     </row>
     <row r="193" spans="1:24">
@@ -9001,8 +9025,8 @@
         <v>208</v>
       </c>
       <c r="X193" t="str">
-        <f>CONCATENATE(A193," ",B193," ",C193," ",D193," ",E193," ",F193," ",G193," ",H193," ",I193," ",J193," ",K193," ",L193," ",M193," ",N193," ",O193," ",P193," ",Q193," ",R193," ",S193," ",U193," ",V193)</f>
-        <v>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_39b --cleanup</v>
+        <f>CONCATENATE(A193," ",B193," ",C193," ",D193," ",E193," ",F193," ",G193," ",H193," ",I193," ",J193," ",K193," ",L193," ",M193," ",N193," ",O193," ",P193," ",Q193," ",R193," ",S193," ",T193," ",U193," ",V193)</f>
+        <v>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_39b --cleanup</v>
       </c>
     </row>
     <row r="194" spans="1:24">
@@ -9118,8 +9142,8 @@
         <v>208</v>
       </c>
       <c r="X197" t="str">
-        <f>CONCATENATE(A197," ",B197," ",C197," ",D197," ",E197," ",F197," ",G197," ",H197," ",I197," ",J197," ",K197," ",L197," ",M197," ",N197," ",O197," ",P197," ",Q197," ",R197," ",S197," ",U197," ",V197)</f>
-        <v>plot_pco_with_stats_all.pl --data_file 16.Qiime.100p.included.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_40w --cleanup</v>
+        <f>CONCATENATE(A197," ",B197," ",C197," ",D197," ",E197," ",F197," ",G197," ",H197," ",I197," ",J197," ",K197," ",L197," ",M197," ",N197," ",O197," ",P197," ",Q197," ",R197," ",S197," ",T197," ",U197," ",V197)</f>
+        <v>plot_pco_with_stats_all.pl --data_file 16.Qiime.100p.included.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_40w --cleanup</v>
       </c>
     </row>
     <row r="198" spans="1:24">
@@ -9190,8 +9214,8 @@
         <v>208</v>
       </c>
       <c r="X198" t="str">
-        <f>CONCATENATE(A198," ",B198," ",C198," ",D198," ",E198," ",F198," ",G198," ",H198," ",I198," ",J198," ",K198," ",L198," ",M198," ",N198," ",O198," ",P198," ",Q198," ",R198," ",S198," ",U198," ",V198)</f>
-        <v>plot_pco_with_stats_all.pl --data_file 16.Qiime.100p.included.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_40b --cleanup</v>
+        <f>CONCATENATE(A198," ",B198," ",C198," ",D198," ",E198," ",F198," ",G198," ",H198," ",I198," ",J198," ",K198," ",L198," ",M198," ",N198," ",O198," ",P198," ",Q198," ",R198," ",S198," ",T198," ",U198," ",V198)</f>
+        <v>plot_pco_with_stats_all.pl --data_file 16.Qiime.100p.included.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_40b --cleanup</v>
       </c>
     </row>
     <row r="199" spans="1:24">
@@ -9307,8 +9331,8 @@
         <v>208</v>
       </c>
       <c r="X202" t="str">
-        <f>CONCATENATE(A202," ",B202," ",C202," ",D202," ",E202," ",F202," ",G202," ",H202," ",I202," ",J202," ",K202," ",L202," ",M202," ",N202," ",O202," ",P202," ",Q202," ",R202," ",S202," ",U202," ",V202)</f>
-        <v>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_41w --cleanup</v>
+        <f>CONCATENATE(A202," ",B202," ",C202," ",D202," ",E202," ",F202," ",G202," ",H202," ",I202," ",J202," ",K202," ",L202," ",M202," ",N202," ",O202," ",P202," ",Q202," ",R202," ",S202," ",T202," ",U202," ",V202)</f>
+        <v>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_41w --cleanup</v>
       </c>
     </row>
     <row r="203" spans="1:24">
@@ -9379,8 +9403,8 @@
         <v>208</v>
       </c>
       <c r="X203" t="str">
-        <f>CONCATENATE(A203," ",B203," ",C203," ",D203," ",E203," ",F203," ",G203," ",H203," ",I203," ",J203," ",K203," ",L203," ",M203," ",N203," ",O203," ",P203," ",Q203," ",R203," ",S203," ",U203," ",V203)</f>
-        <v>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_41b --cleanup</v>
+        <f>CONCATENATE(A203," ",B203," ",C203," ",D203," ",E203," ",F203," ",G203," ",H203," ",I203," ",J203," ",K203," ",L203," ",M203," ",N203," ",O203," ",P203," ",Q203," ",R203," ",S203," ",T203," ",U203," ",V203)</f>
+        <v>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_41b --cleanup</v>
       </c>
     </row>
     <row r="204" spans="1:24">
@@ -9496,8 +9520,8 @@
         <v>208</v>
       </c>
       <c r="X207" t="str">
-        <f>CONCATENATE(A207," ",B207," ",C207," ",D207," ",E207," ",F207," ",G207," ",H207," ",I207," ",J207," ",K207," ",L207," ",M207," ",N207," ",O207," ",P207," ",Q207," ",R207," ",S207," ",U207," ",V207)</f>
-        <v>plot_pco_with_stats_all.pl --data_file 14.Qiime.100p.removed.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_42w --cleanup</v>
+        <f>CONCATENATE(A207," ",B207," ",C207," ",D207," ",E207," ",F207," ",G207," ",H207," ",I207," ",J207," ",K207," ",L207," ",M207," ",N207," ",O207," ",P207," ",Q207," ",R207," ",S207," ",T207," ",U207," ",V207)</f>
+        <v>plot_pco_with_stats_all.pl --data_file 14.Qiime.100p.removed.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_42w --cleanup</v>
       </c>
     </row>
     <row r="208" spans="1:24">
@@ -9568,8 +9592,8 @@
         <v>208</v>
       </c>
       <c r="X208" t="str">
-        <f>CONCATENATE(A208," ",B208," ",C208," ",D208," ",E208," ",F208," ",G208," ",H208," ",I208," ",J208," ",K208," ",L208," ",M208," ",N208," ",O208," ",P208," ",Q208," ",R208," ",S208," ",U208," ",V208)</f>
-        <v>plot_pco_with_stats_all.pl --data_file 14.Qiime.100p.removed.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_42b --cleanup</v>
+        <f>CONCATENATE(A208," ",B208," ",C208," ",D208," ",E208," ",F208," ",G208," ",H208," ",I208," ",J208," ",K208," ",L208," ",M208," ",N208," ",O208," ",P208," ",Q208," ",R208," ",S208," ",T208," ",U208," ",V208)</f>
+        <v>plot_pco_with_stats_all.pl --data_file 14.Qiime.100p.removed.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_42b --cleanup</v>
       </c>
     </row>
     <row r="209" spans="1:24">
@@ -9685,8 +9709,8 @@
         <v>208</v>
       </c>
       <c r="X212" t="str">
-        <f>CONCATENATE(A212," ",B212," ",C212," ",D212," ",E212," ",F212," ",G212," ",H212," ",I212," ",J212," ",K212," ",L212," ",M212," ",N212," ",O212," ",P212," ",Q212," ",R212," ",S212," ",U212," ",V212)</f>
-        <v>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_43w --cleanup</v>
+        <f>CONCATENATE(A212," ",B212," ",C212," ",D212," ",E212," ",F212," ",G212," ",H212," ",I212," ",J212," ",K212," ",L212," ",M212," ",N212," ",O212," ",P212," ",Q212," ",R212," ",S212," ",T212," ",U212," ",V212)</f>
+        <v>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_43w --cleanup</v>
       </c>
     </row>
     <row r="213" spans="1:24">
@@ -9757,8 +9781,8 @@
         <v>208</v>
       </c>
       <c r="X213" t="str">
-        <f>CONCATENATE(A213," ",B213," ",C213," ",D213," ",E213," ",F213," ",G213," ",H213," ",I213," ",J213," ",K213," ",L213," ",M213," ",N213," ",O213," ",P213," ",Q213," ",R213," ",S213," ",U213," ",V213)</f>
-        <v>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_43b --cleanup</v>
+        <f>CONCATENATE(A213," ",B213," ",C213," ",D213," ",E213," ",F213," ",G213," ",H213," ",I213," ",J213," ",K213," ",L213," ",M213," ",N213," ",O213," ",P213," ",Q213," ",R213," ",S213," ",T213," ",U213," ",V213)</f>
+        <v>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_43b --cleanup</v>
       </c>
     </row>
     <row r="214" spans="1:24">
@@ -9874,8 +9898,8 @@
         <v>208</v>
       </c>
       <c r="X217" t="str">
-        <f>CONCATENATE(A217," ",B217," ",C217," ",D217," ",E217," ",F217," ",G217," ",H217," ",I217," ",J217," ",K217," ",L217," ",M217," ",N217," ",O217," ",P217," ",Q217," ",R217," ",S217," ",U217," ",V217)</f>
-        <v>plot_pco_with_stats_all.pl --data_file 16.Qiime.100p.included.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_44w --cleanup</v>
+        <f>CONCATENATE(A217," ",B217," ",C217," ",D217," ",E217," ",F217," ",G217," ",H217," ",I217," ",J217," ",K217," ",L217," ",M217," ",N217," ",O217," ",P217," ",Q217," ",R217," ",S217," ",T217," ",U217," ",V217)</f>
+        <v>plot_pco_with_stats_all.pl --data_file 16.Qiime.100p.included.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_44w --cleanup</v>
       </c>
     </row>
     <row r="218" spans="1:24">
@@ -9946,8 +9970,8 @@
         <v>208</v>
       </c>
       <c r="X218" t="str">
-        <f>CONCATENATE(A218," ",B218," ",C218," ",D218," ",E218," ",F218," ",G218," ",H218," ",I218," ",J218," ",K218," ",L218," ",M218," ",N218," ",O218," ",P218," ",Q218," ",R218," ",S218," ",U218," ",V218)</f>
-        <v>plot_pco_with_stats_all.pl --data_file 16.Qiime.100p.included.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_44b --cleanup</v>
+        <f>CONCATENATE(A218," ",B218," ",C218," ",D218," ",E218," ",F218," ",G218," ",H218," ",I218," ",J218," ",K218," ",L218," ",M218," ",N218," ",O218," ",P218," ",Q218," ",R218," ",S218," ",T218," ",U218," ",V218)</f>
+        <v>plot_pco_with_stats_all.pl --data_file 16.Qiime.100p.included.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_44b --cleanup</v>
       </c>
     </row>
     <row r="219" spans="1:24">
@@ -10063,8 +10087,8 @@
         <v>208</v>
       </c>
       <c r="X222" t="str">
-        <f>CONCATENATE(A222," ",B222," ",C222," ",D222," ",E222," ",F222," ",G222," ",H222," ",I222," ",J222," ",K222," ",L222," ",M222," ",N222," ",O222," ",P222," ",Q222," ",R222," ",S222," ",U222," ",V222)</f>
-        <v>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_45w --cleanup</v>
+        <f>CONCATENATE(A222," ",B222," ",C222," ",D222," ",E222," ",F222," ",G222," ",H222," ",I222," ",J222," ",K222," ",L222," ",M222," ",N222," ",O222," ",P222," ",Q222," ",R222," ",S222," ",T222," ",U222," ",V222)</f>
+        <v>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_45w --cleanup</v>
       </c>
     </row>
     <row r="223" spans="1:24">
@@ -10135,8 +10159,8 @@
         <v>208</v>
       </c>
       <c r="X223" t="str">
-        <f>CONCATENATE(A223," ",B223," ",C223," ",D223," ",E223," ",F223," ",G223," ",H223," ",I223," ",J223," ",K223," ",L223," ",M223," ",N223," ",O223," ",P223," ",Q223," ",R223," ",S223," ",U223," ",V223)</f>
-        <v>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_45b --cleanup</v>
+        <f>CONCATENATE(A223," ",B223," ",C223," ",D223," ",E223," ",F223," ",G223," ",H223," ",I223," ",J223," ",K223," ",L223," ",M223," ",N223," ",O223," ",P223," ",Q223," ",R223," ",S223," ",T223," ",U223," ",V223)</f>
+        <v>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_45b --cleanup</v>
       </c>
     </row>
     <row r="224" spans="1:24">
@@ -10252,8 +10276,8 @@
         <v>208</v>
       </c>
       <c r="X227" t="str">
-        <f>CONCATENATE(A227," ",B227," ",C227," ",D227," ",E227," ",F227," ",G227," ",H227," ",I227," ",J227," ",K227," ",L227," ",M227," ",N227," ",O227," ",P227," ",Q227," ",R227," ",S227," ",U227," ",V227)</f>
-        <v>plot_pco_with_stats_all.pl --data_file 14.Qiime.100p.removed.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_46w --cleanup</v>
+        <f>CONCATENATE(A227," ",B227," ",C227," ",D227," ",E227," ",F227," ",G227," ",H227," ",I227," ",J227," ",K227," ",L227," ",M227," ",N227," ",O227," ",P227," ",Q227," ",R227," ",S227," ",T227," ",U227," ",V227)</f>
+        <v>plot_pco_with_stats_all.pl --data_file 14.Qiime.100p.removed.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_46w --cleanup</v>
       </c>
     </row>
     <row r="228" spans="1:24">
@@ -10324,8 +10348,8 @@
         <v>208</v>
       </c>
       <c r="X228" t="str">
-        <f>CONCATENATE(A228," ",B228," ",C228," ",D228," ",E228," ",F228," ",G228," ",H228," ",I228," ",J228," ",K228," ",L228," ",M228," ",N228," ",O228," ",P228," ",Q228," ",R228," ",S228," ",U228," ",V228)</f>
-        <v>plot_pco_with_stats_all.pl --data_file 14.Qiime.100p.removed.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 Analysis_46b --cleanup</v>
+        <f>CONCATENATE(A228," ",B228," ",C228," ",D228," ",E228," ",F228," ",G228," ",H228," ",I228," ",J228," ",K228," ",L228," ",M228," ",N228," ",O228," ",P228," ",Q228," ",R228," ",S228," ",T228," ",U228," ",V228)</f>
+        <v>plot_pco_with_stats_all.pl --data_file 14.Qiime.100p.removed.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_46b --cleanup</v>
       </c>
     </row>
     <row r="229" spans="1:24">
@@ -10363,7 +10387,7 @@
     </row>
     <row r="230" spans="1:24">
       <c r="X230" t="str">
-        <f t="shared" ref="X200:X260" si="3">CONCATENATE(A230," ",B230," ",C230," ",D230," ",E230," ",F230," ",G230," ",H230," ",I230," ",J230," ",K230," ",L230," ",M230," ",N230," ",O230," ",P230," ",Q230," ",R230," ",S230," ",T230," ",U230," ",V230)</f>
+        <f t="shared" ref="X230:X260" si="3">CONCATENATE(A230," ",B230," ",C230," ",D230," ",E230," ",F230," ",G230," ",H230," ",I230," ",J230," ",K230," ",L230," ",M230," ",N230," ",O230," ",P230," ",Q230," ",R230," ",S230," ",T230," ",U230," ",V230)</f>
         <v xml:space="preserve">                     </v>
       </c>
     </row>
@@ -10447,7 +10471,7 @@
         <v>208</v>
       </c>
       <c r="X232" t="str">
-        <f t="shared" si="3"/>
+        <f>CONCATENATE(A232," ",B232," ",C232," ",D232," ",E232," ",F232," ",G232," ",H232," ",I232," ",J232," ",K232," ",L232," ",M232," ",N232," ",O232," ",P232," ",Q232," ",R232," ",S232," ",T232," ",U232," ",V232)</f>
         <v>plot_pco_with_stats_all.pl --data_file 11.Qiime.Qiime_default.included.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_47w --cleanup</v>
       </c>
     </row>
@@ -10519,7 +10543,7 @@
         <v>208</v>
       </c>
       <c r="X233" t="str">
-        <f t="shared" si="3"/>
+        <f>CONCATENATE(A233," ",B233," ",C233," ",D233," ",E233," ",F233," ",G233," ",H233," ",I233," ",J233," ",K233," ",L233," ",M233," ",N233," ",O233," ",P233," ",Q233," ",R233," ",S233," ",T233," ",U233," ",V233)</f>
         <v>plot_pco_with_stats_all.pl --data_file 11.Qiime.Qiime_default.included.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_47b --cleanup</v>
       </c>
     </row>
@@ -10642,7 +10666,7 @@
         <v>208</v>
       </c>
       <c r="X237" t="str">
-        <f t="shared" si="3"/>
+        <f>CONCATENATE(A237," ",B237," ",C237," ",D237," ",E237," ",F237," ",G237," ",H237," ",I237," ",J237," ",K237," ",L237," ",M237," ",N237," ",O237," ",P237," ",Q237," ",R237," ",S237," ",T237," ",U237," ",V237)</f>
         <v>plot_pco_with_stats_all.pl --data_file 11.Qiime.Qiime_default.included.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_48w --cleanup</v>
       </c>
     </row>
@@ -10714,7 +10738,7 @@
         <v>208</v>
       </c>
       <c r="X238" t="str">
-        <f t="shared" si="3"/>
+        <f>CONCATENATE(A238," ",B238," ",C238," ",D238," ",E238," ",F238," ",G238," ",H238," ",I238," ",J238," ",K238," ",L238," ",M238," ",N238," ",O238," ",P238," ",Q238," ",R238," ",S238," ",T238," ",U238," ",V238)</f>
         <v>plot_pco_with_stats_all.pl --data_file 11.Qiime.Qiime_default.included.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_48b --cleanup</v>
       </c>
     </row>
@@ -10837,7 +10861,7 @@
         <v>208</v>
       </c>
       <c r="X242" t="str">
-        <f t="shared" si="3"/>
+        <f>CONCATENATE(A242," ",B242," ",C242," ",D242," ",E242," ",F242," ",G242," ",H242," ",I242," ",J242," ",K242," ",L242," ",M242," ",N242," ",O242," ",P242," ",Q242," ",R242," ",S242," ",T242," ",U242," ",V242)</f>
         <v>plot_pco_with_stats_all.pl --data_file 9.Qiime.Qiime_default.removed.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_49w --cleanup</v>
       </c>
     </row>
@@ -10909,7 +10933,7 @@
         <v>208</v>
       </c>
       <c r="X243" t="str">
-        <f t="shared" si="3"/>
+        <f>CONCATENATE(A243," ",B243," ",C243," ",D243," ",E243," ",F243," ",G243," ",H243," ",I243," ",J243," ",K243," ",L243," ",M243," ",N243," ",O243," ",P243," ",Q243," ",R243," ",S243," ",T243," ",U243," ",V243)</f>
         <v>plot_pco_with_stats_all.pl --data_file 9.Qiime.Qiime_default.removed.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_49b --cleanup</v>
       </c>
     </row>
@@ -11032,7 +11056,7 @@
         <v>208</v>
       </c>
       <c r="X247" t="str">
-        <f t="shared" si="3"/>
+        <f>CONCATENATE(A247," ",B247," ",C247," ",D247," ",E247," ",F247," ",G247," ",H247," ",I247," ",J247," ",K247," ",L247," ",M247," ",N247," ",O247," ",P247," ",Q247," ",R247," ",S247," ",T247," ",U247," ",V247)</f>
         <v>plot_pco_with_stats_all.pl --data_file 9.Qiime.Qiime_default.removed.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_50w --cleanup</v>
       </c>
     </row>
@@ -11104,7 +11128,7 @@
         <v>208</v>
       </c>
       <c r="X248" t="str">
-        <f t="shared" si="3"/>
+        <f>CONCATENATE(A248," ",B248," ",C248," ",D248," ",E248," ",F248," ",G248," ",H248," ",I248," ",J248," ",K248," ",L248," ",M248," ",N248," ",O248," ",P248," ",Q248," ",R248," ",S248," ",T248," ",U248," ",V248)</f>
         <v>plot_pco_with_stats_all.pl --data_file 9.Qiime.Qiime_default.removed.raw --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_50b --cleanup</v>
       </c>
     </row>
@@ -11227,7 +11251,7 @@
         <v>208</v>
       </c>
       <c r="X252" t="str">
-        <f t="shared" si="3"/>
+        <f>CONCATENATE(A252," ",B252," ",C252," ",D252," ",E252," ",F252," ",G252," ",H252," ",I252," ",J252," ",K252," ",L252," ",M252," ",N252," ",O252," ",P252," ",Q252," ",R252," ",S252," ",T252," ",U252," ",V252)</f>
         <v>plot_pco_with_stats_all.pl --data_file 12.Qiime.Qiime_default.included.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_51w --cleanup</v>
       </c>
     </row>
@@ -11299,7 +11323,7 @@
         <v>208</v>
       </c>
       <c r="X253" t="str">
-        <f t="shared" si="3"/>
+        <f>CONCATENATE(A253," ",B253," ",C253," ",D253," ",E253," ",F253," ",G253," ",H253," ",I253," ",J253," ",K253," ",L253," ",M253," ",N253," ",O253," ",P253," ",Q253," ",R253," ",S253," ",T253," ",U253," ",V253)</f>
         <v>plot_pco_with_stats_all.pl --data_file 12.Qiime.Qiime_default.included.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_51b --cleanup</v>
       </c>
     </row>
@@ -11422,7 +11446,7 @@
         <v>208</v>
       </c>
       <c r="X257" t="str">
-        <f t="shared" si="3"/>
+        <f>CONCATENATE(A257," ",B257," ",C257," ",D257," ",E257," ",F257," ",G257," ",H257," ",I257," ",J257," ",K257," ",L257," ",M257," ",N257," ",O257," ",P257," ",Q257," ",R257," ",S257," ",T257," ",U257," ",V257)</f>
         <v>plot_pco_with_stats_all.pl --data_file 12.Qiime.Qiime_default.included.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_52w --cleanup</v>
       </c>
     </row>
@@ -11494,7 +11518,7 @@
         <v>208</v>
       </c>
       <c r="X258" t="str">
-        <f t="shared" si="3"/>
+        <f>CONCATENATE(A258," ",B258," ",C258," ",D258," ",E258," ",F258," ",G258," ",H258," ",I258," ",J258," ",K258," ",L258," ",M258," ",N258," ",O258," ",P258," ",Q258," ",R258," ",S258," ",T258," ",U258," ",V258)</f>
         <v>plot_pco_with_stats_all.pl --data_file 12.Qiime.Qiime_default.included.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_52b --cleanup</v>
       </c>
     </row>
@@ -11617,7 +11641,7 @@
         <v>208</v>
       </c>
       <c r="X262" t="str">
-        <f t="shared" ref="X262:X268" si="4">CONCATENATE(A262," ",B262," ",C262," ",D262," ",E262," ",F262," ",G262," ",H262," ",I262," ",J262," ",K262," ",L262," ",M262," ",N262," ",O262," ",P262," ",Q262," ",R262," ",S262," ",T262," ",U262," ",V262)</f>
+        <f>CONCATENATE(A262," ",B262," ",C262," ",D262," ",E262," ",F262," ",G262," ",H262," ",I262," ",J262," ",K262," ",L262," ",M262," ",N262," ",O262," ",P262," ",Q262," ",R262," ",S262," ",T262," ",U262," ",V262)</f>
         <v>plot_pco_with_stats_all.pl --data_file 10.Qiime.Qiime_default.removed.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_53w --cleanup</v>
       </c>
     </row>
@@ -11689,7 +11713,7 @@
         <v>208</v>
       </c>
       <c r="X263" t="str">
-        <f t="shared" si="4"/>
+        <f>CONCATENATE(A263," ",B263," ",C263," ",D263," ",E263," ",F263," ",G263," ",H263," ",I263," ",J263," ",K263," ",L263," ",M263," ",N263," ",O263," ",P263," ",Q263," ",R263," ",S263," ",T263," ",U263," ",V263)</f>
         <v>plot_pco_with_stats_all.pl --data_file 10.Qiime.Qiime_default.removed.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_53b --cleanup</v>
       </c>
     </row>
@@ -11728,7 +11752,7 @@
     </row>
     <row r="265" spans="1:24">
       <c r="X265" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="X262:X267" si="4">CONCATENATE(A265," ",B265," ",C265," ",D265," ",E265," ",F265," ",G265," ",H265," ",I265," ",J265," ",K265," ",L265," ",M265," ",N265," ",O265," ",P265," ",Q265," ",R265," ",S265," ",T265," ",U265," ",V265)</f>
         <v xml:space="preserve">                     </v>
       </c>
     </row>
@@ -11812,7 +11836,7 @@
         <v>208</v>
       </c>
       <c r="X267" t="str">
-        <f t="shared" si="4"/>
+        <f>CONCATENATE(A267," ",B267," ",C267," ",D267," ",E267," ",F267," ",G267," ",H267," ",I267," ",J267," ",K267," ",L267," ",M267," ",N267," ",O267," ",P267," ",Q267," ",R267," ",S267," ",T267," ",U267," ",V267)</f>
         <v>plot_pco_with_stats_all.pl --data_file 10.Qiime.Qiime_default.removed.norm --groups_list AMETHST.stat.groups --num_perm 1000 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree ~/AMETHST/qiime_trees/97_otus.tree --num_cpus 10 --output_prefix Analysis_54w --cleanup</v>
       </c>
     </row>
@@ -11949,12 +11973,12 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>434</v>
+        <v>378</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>435</v>
+        <v>379</v>
       </c>
     </row>
     <row r="4" spans="1:1">
@@ -11974,12 +11998,12 @@
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>436</v>
+        <v>380</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>437</v>
+        <v>381</v>
       </c>
     </row>
     <row r="9" spans="1:1">
@@ -11999,12 +12023,12 @@
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>438</v>
+        <v>382</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>439</v>
+        <v>383</v>
       </c>
     </row>
     <row r="14" spans="1:1">
@@ -12024,12 +12048,12 @@
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>440</v>
+        <v>384</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>441</v>
+        <v>385</v>
       </c>
     </row>
     <row r="19" spans="1:1">
@@ -12124,12 +12148,12 @@
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>442</v>
+        <v>386</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>443</v>
+        <v>387</v>
       </c>
     </row>
     <row r="39" spans="1:1">
@@ -12144,12 +12168,12 @@
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>444</v>
+        <v>388</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>445</v>
+        <v>389</v>
       </c>
     </row>
     <row r="44" spans="1:1">
@@ -12164,12 +12188,12 @@
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>446</v>
+        <v>390</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>447</v>
+        <v>391</v>
       </c>
     </row>
     <row r="49" spans="1:1">
@@ -12184,12 +12208,12 @@
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="s">
-        <v>448</v>
+        <v>392</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>449</v>
+        <v>393</v>
       </c>
     </row>
     <row r="54" spans="1:1">
@@ -12284,12 +12308,12 @@
     </row>
     <row r="72" spans="1:1">
       <c r="A72" t="s">
-        <v>450</v>
+        <v>394</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" t="s">
-        <v>451</v>
+        <v>395</v>
       </c>
     </row>
     <row r="74" spans="1:1">
@@ -12304,12 +12328,12 @@
     </row>
     <row r="77" spans="1:1">
       <c r="A77" t="s">
-        <v>452</v>
+        <v>396</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" t="s">
-        <v>453</v>
+        <v>397</v>
       </c>
     </row>
     <row r="79" spans="1:1">
@@ -12324,12 +12348,12 @@
     </row>
     <row r="82" spans="1:1">
       <c r="A82" t="s">
-        <v>454</v>
+        <v>398</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" t="s">
-        <v>455</v>
+        <v>399</v>
       </c>
     </row>
     <row r="84" spans="1:1">
@@ -12344,12 +12368,12 @@
     </row>
     <row r="87" spans="1:1">
       <c r="A87" t="s">
-        <v>456</v>
+        <v>400</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" t="s">
-        <v>457</v>
+        <v>401</v>
       </c>
     </row>
     <row r="89" spans="1:1">
@@ -12369,17 +12393,17 @@
     </row>
     <row r="92" spans="1:1">
       <c r="A92" t="s">
-        <v>298</v>
+        <v>484</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" t="s">
-        <v>299</v>
+        <v>482</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="96" spans="1:1">
@@ -12389,17 +12413,17 @@
     </row>
     <row r="97" spans="1:1">
       <c r="A97" t="s">
-        <v>301</v>
+        <v>485</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" t="s">
-        <v>302</v>
+        <v>486</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="101" spans="1:1">
@@ -12409,17 +12433,17 @@
     </row>
     <row r="102" spans="1:1">
       <c r="A102" t="s">
-        <v>304</v>
+        <v>487</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" t="s">
-        <v>305</v>
+        <v>488</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
     </row>
     <row r="105" spans="1:1">
@@ -12434,17 +12458,17 @@
     </row>
     <row r="107" spans="1:1">
       <c r="A107" t="s">
-        <v>458</v>
+        <v>402</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108" t="s">
-        <v>459</v>
+        <v>403</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="111" spans="1:1">
@@ -12454,17 +12478,17 @@
     </row>
     <row r="112" spans="1:1">
       <c r="A112" t="s">
-        <v>460</v>
+        <v>404</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" t="s">
-        <v>461</v>
+        <v>405</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
     </row>
     <row r="116" spans="1:1">
@@ -12474,17 +12498,17 @@
     </row>
     <row r="117" spans="1:1">
       <c r="A117" t="s">
-        <v>462</v>
+        <v>406</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" t="s">
-        <v>463</v>
+        <v>407</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
     </row>
     <row r="121" spans="1:1">
@@ -12494,17 +12518,17 @@
     </row>
     <row r="122" spans="1:1">
       <c r="A122" t="s">
-        <v>464</v>
+        <v>408</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" t="s">
-        <v>465</v>
+        <v>409</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
     </row>
     <row r="125" spans="1:1">
@@ -12519,17 +12543,17 @@
     </row>
     <row r="127" spans="1:1">
       <c r="A127" t="s">
-        <v>311</v>
+        <v>483</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128" t="s">
-        <v>312</v>
+        <v>489</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
     </row>
     <row r="131" spans="1:1">
@@ -12539,17 +12563,17 @@
     </row>
     <row r="132" spans="1:1">
       <c r="A132" t="s">
-        <v>314</v>
+        <v>490</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133" t="s">
-        <v>315</v>
+        <v>491</v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
     </row>
     <row r="136" spans="1:1">
@@ -12559,17 +12583,17 @@
     </row>
     <row r="137" spans="1:1">
       <c r="A137" t="s">
-        <v>317</v>
+        <v>492</v>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138" t="s">
-        <v>318</v>
+        <v>493</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139" t="s">
-        <v>319</v>
+        <v>307</v>
       </c>
     </row>
     <row r="140" spans="1:1">
@@ -12584,17 +12608,17 @@
     </row>
     <row r="142" spans="1:1">
       <c r="A142" t="s">
-        <v>466</v>
+        <v>410</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143" t="s">
-        <v>467</v>
+        <v>411</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144" t="s">
-        <v>320</v>
+        <v>308</v>
       </c>
     </row>
     <row r="146" spans="1:1">
@@ -12604,17 +12628,17 @@
     </row>
     <row r="147" spans="1:1">
       <c r="A147" t="s">
-        <v>468</v>
+        <v>412</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148" t="s">
-        <v>469</v>
+        <v>413</v>
       </c>
     </row>
     <row r="149" spans="1:1">
       <c r="A149" t="s">
-        <v>321</v>
+        <v>309</v>
       </c>
     </row>
     <row r="151" spans="1:1">
@@ -12624,17 +12648,17 @@
     </row>
     <row r="152" spans="1:1">
       <c r="A152" t="s">
-        <v>470</v>
+        <v>414</v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153" t="s">
-        <v>471</v>
+        <v>415</v>
       </c>
     </row>
     <row r="154" spans="1:1">
       <c r="A154" t="s">
-        <v>322</v>
+        <v>310</v>
       </c>
     </row>
     <row r="156" spans="1:1">
@@ -12644,17 +12668,17 @@
     </row>
     <row r="157" spans="1:1">
       <c r="A157" t="s">
-        <v>472</v>
+        <v>416</v>
       </c>
     </row>
     <row r="158" spans="1:1">
       <c r="A158" t="s">
-        <v>473</v>
+        <v>417</v>
       </c>
     </row>
     <row r="159" spans="1:1">
       <c r="A159" t="s">
-        <v>323</v>
+        <v>311</v>
       </c>
     </row>
     <row r="161" spans="1:1">
@@ -12664,17 +12688,17 @@
     </row>
     <row r="162" spans="1:1">
       <c r="A162" t="s">
-        <v>474</v>
+        <v>418</v>
       </c>
     </row>
     <row r="163" spans="1:1">
       <c r="A163" t="s">
-        <v>475</v>
+        <v>419</v>
       </c>
     </row>
     <row r="164" spans="1:1">
       <c r="A164" t="s">
-        <v>324</v>
+        <v>312</v>
       </c>
     </row>
     <row r="166" spans="1:1">
@@ -12684,17 +12708,17 @@
     </row>
     <row r="167" spans="1:1">
       <c r="A167" t="s">
-        <v>476</v>
+        <v>420</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168" t="s">
-        <v>477</v>
+        <v>421</v>
       </c>
     </row>
     <row r="169" spans="1:1">
       <c r="A169" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
     </row>
     <row r="171" spans="1:1">
@@ -12704,17 +12728,17 @@
     </row>
     <row r="172" spans="1:1">
       <c r="A172" t="s">
-        <v>478</v>
+        <v>422</v>
       </c>
     </row>
     <row r="173" spans="1:1">
       <c r="A173" t="s">
-        <v>479</v>
+        <v>423</v>
       </c>
     </row>
     <row r="174" spans="1:1">
       <c r="A174" t="s">
-        <v>326</v>
+        <v>314</v>
       </c>
     </row>
     <row r="176" spans="1:1">
@@ -12724,17 +12748,17 @@
     </row>
     <row r="177" spans="1:1">
       <c r="A177" t="s">
-        <v>480</v>
+        <v>424</v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178" t="s">
-        <v>481</v>
+        <v>425</v>
       </c>
     </row>
     <row r="179" spans="1:1">
       <c r="A179" t="s">
-        <v>327</v>
+        <v>315</v>
       </c>
     </row>
     <row r="181" spans="1:1">
@@ -12744,17 +12768,17 @@
     </row>
     <row r="182" spans="1:1">
       <c r="A182" t="s">
-        <v>482</v>
+        <v>426</v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183" t="s">
-        <v>483</v>
+        <v>427</v>
       </c>
     </row>
     <row r="184" spans="1:1">
       <c r="A184" t="s">
-        <v>328</v>
+        <v>316</v>
       </c>
     </row>
     <row r="186" spans="1:1">
@@ -12764,17 +12788,17 @@
     </row>
     <row r="187" spans="1:1">
       <c r="A187" t="s">
-        <v>484</v>
+        <v>428</v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188" t="s">
-        <v>485</v>
+        <v>429</v>
       </c>
     </row>
     <row r="189" spans="1:1">
       <c r="A189" t="s">
-        <v>329</v>
+        <v>317</v>
       </c>
     </row>
     <row r="190" spans="1:1">
@@ -12789,17 +12813,17 @@
     </row>
     <row r="192" spans="1:1">
       <c r="A192" t="s">
-        <v>330</v>
+        <v>494</v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193" t="s">
-        <v>331</v>
+        <v>495</v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194" t="s">
-        <v>332</v>
+        <v>318</v>
       </c>
     </row>
     <row r="196" spans="1:1">
@@ -12809,17 +12833,17 @@
     </row>
     <row r="197" spans="1:1">
       <c r="A197" t="s">
-        <v>333</v>
+        <v>496</v>
       </c>
     </row>
     <row r="198" spans="1:1">
       <c r="A198" t="s">
-        <v>334</v>
+        <v>497</v>
       </c>
     </row>
     <row r="199" spans="1:1">
       <c r="A199" t="s">
-        <v>335</v>
+        <v>319</v>
       </c>
     </row>
     <row r="201" spans="1:1">
@@ -12829,17 +12853,17 @@
     </row>
     <row r="202" spans="1:1">
       <c r="A202" t="s">
-        <v>336</v>
+        <v>498</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203" t="s">
-        <v>337</v>
+        <v>499</v>
       </c>
     </row>
     <row r="204" spans="1:1">
       <c r="A204" t="s">
-        <v>338</v>
+        <v>320</v>
       </c>
     </row>
     <row r="206" spans="1:1">
@@ -12849,17 +12873,17 @@
     </row>
     <row r="207" spans="1:1">
       <c r="A207" t="s">
-        <v>339</v>
+        <v>500</v>
       </c>
     </row>
     <row r="208" spans="1:1">
       <c r="A208" t="s">
-        <v>340</v>
+        <v>501</v>
       </c>
     </row>
     <row r="209" spans="1:1">
       <c r="A209" t="s">
-        <v>341</v>
+        <v>321</v>
       </c>
     </row>
     <row r="211" spans="1:1">
@@ -12869,17 +12893,17 @@
     </row>
     <row r="212" spans="1:1">
       <c r="A212" t="s">
-        <v>342</v>
+        <v>502</v>
       </c>
     </row>
     <row r="213" spans="1:1">
       <c r="A213" t="s">
-        <v>343</v>
+        <v>503</v>
       </c>
     </row>
     <row r="214" spans="1:1">
       <c r="A214" t="s">
-        <v>344</v>
+        <v>322</v>
       </c>
     </row>
     <row r="216" spans="1:1">
@@ -12889,17 +12913,17 @@
     </row>
     <row r="217" spans="1:1">
       <c r="A217" t="s">
-        <v>345</v>
+        <v>504</v>
       </c>
     </row>
     <row r="218" spans="1:1">
       <c r="A218" t="s">
-        <v>346</v>
+        <v>505</v>
       </c>
     </row>
     <row r="219" spans="1:1">
       <c r="A219" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
     </row>
     <row r="221" spans="1:1">
@@ -12909,17 +12933,17 @@
     </row>
     <row r="222" spans="1:1">
       <c r="A222" t="s">
-        <v>348</v>
+        <v>506</v>
       </c>
     </row>
     <row r="223" spans="1:1">
       <c r="A223" t="s">
-        <v>349</v>
+        <v>507</v>
       </c>
     </row>
     <row r="224" spans="1:1">
       <c r="A224" t="s">
-        <v>350</v>
+        <v>324</v>
       </c>
     </row>
     <row r="226" spans="1:1">
@@ -12929,17 +12953,17 @@
     </row>
     <row r="227" spans="1:1">
       <c r="A227" t="s">
-        <v>351</v>
+        <v>508</v>
       </c>
     </row>
     <row r="228" spans="1:1">
       <c r="A228" t="s">
-        <v>352</v>
+        <v>509</v>
       </c>
     </row>
     <row r="229" spans="1:1">
       <c r="A229" t="s">
-        <v>353</v>
+        <v>325</v>
       </c>
     </row>
     <row r="230" spans="1:1">
@@ -12954,17 +12978,17 @@
     </row>
     <row r="232" spans="1:1">
       <c r="A232" t="s">
-        <v>354</v>
+        <v>326</v>
       </c>
     </row>
     <row r="233" spans="1:1">
       <c r="A233" t="s">
-        <v>355</v>
+        <v>327</v>
       </c>
     </row>
     <row r="234" spans="1:1">
       <c r="A234" t="s">
-        <v>356</v>
+        <v>328</v>
       </c>
     </row>
     <row r="235" spans="1:1">
@@ -12979,17 +13003,17 @@
     </row>
     <row r="237" spans="1:1">
       <c r="A237" t="s">
-        <v>357</v>
+        <v>329</v>
       </c>
     </row>
     <row r="238" spans="1:1">
       <c r="A238" t="s">
-        <v>358</v>
+        <v>330</v>
       </c>
     </row>
     <row r="239" spans="1:1">
       <c r="A239" t="s">
-        <v>359</v>
+        <v>331</v>
       </c>
     </row>
     <row r="240" spans="1:1">
@@ -13004,17 +13028,17 @@
     </row>
     <row r="242" spans="1:1">
       <c r="A242" t="s">
-        <v>360</v>
+        <v>332</v>
       </c>
     </row>
     <row r="243" spans="1:1">
       <c r="A243" t="s">
-        <v>361</v>
+        <v>333</v>
       </c>
     </row>
     <row r="244" spans="1:1">
       <c r="A244" t="s">
-        <v>362</v>
+        <v>334</v>
       </c>
     </row>
     <row r="245" spans="1:1">
@@ -13029,17 +13053,17 @@
     </row>
     <row r="247" spans="1:1">
       <c r="A247" t="s">
-        <v>363</v>
+        <v>335</v>
       </c>
     </row>
     <row r="248" spans="1:1">
       <c r="A248" t="s">
-        <v>364</v>
+        <v>336</v>
       </c>
     </row>
     <row r="249" spans="1:1">
       <c r="A249" t="s">
-        <v>365</v>
+        <v>337</v>
       </c>
     </row>
     <row r="250" spans="1:1">
@@ -13054,17 +13078,17 @@
     </row>
     <row r="252" spans="1:1">
       <c r="A252" t="s">
-        <v>366</v>
+        <v>338</v>
       </c>
     </row>
     <row r="253" spans="1:1">
       <c r="A253" t="s">
-        <v>367</v>
+        <v>339</v>
       </c>
     </row>
     <row r="254" spans="1:1">
       <c r="A254" t="s">
-        <v>368</v>
+        <v>340</v>
       </c>
     </row>
     <row r="255" spans="1:1">
@@ -13079,17 +13103,17 @@
     </row>
     <row r="257" spans="1:1">
       <c r="A257" t="s">
-        <v>369</v>
+        <v>341</v>
       </c>
     </row>
     <row r="258" spans="1:1">
       <c r="A258" t="s">
-        <v>370</v>
+        <v>342</v>
       </c>
     </row>
     <row r="259" spans="1:1">
       <c r="A259" t="s">
-        <v>371</v>
+        <v>343</v>
       </c>
     </row>
     <row r="260" spans="1:1">
@@ -13104,17 +13128,17 @@
     </row>
     <row r="262" spans="1:1">
       <c r="A262" t="s">
-        <v>372</v>
+        <v>344</v>
       </c>
     </row>
     <row r="263" spans="1:1">
       <c r="A263" t="s">
-        <v>373</v>
+        <v>345</v>
       </c>
     </row>
     <row r="264" spans="1:1">
       <c r="A264" t="s">
-        <v>374</v>
+        <v>346</v>
       </c>
     </row>
     <row r="265" spans="1:1">
@@ -13129,17 +13153,17 @@
     </row>
     <row r="267" spans="1:1">
       <c r="A267" t="s">
-        <v>375</v>
+        <v>347</v>
       </c>
     </row>
     <row r="268" spans="1:1">
       <c r="A268" t="s">
-        <v>376</v>
+        <v>348</v>
       </c>
     </row>
     <row r="269" spans="1:1">
       <c r="A269" t="s">
-        <v>377</v>
+        <v>349</v>
       </c>
     </row>
   </sheetData>
@@ -13157,7 +13181,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A269"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A210" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
       <selection activeCell="A210" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
@@ -13170,12 +13194,12 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>486</v>
+        <v>430</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>487</v>
+        <v>431</v>
       </c>
     </row>
     <row r="4" spans="1:1">
@@ -13195,12 +13219,12 @@
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>488</v>
+        <v>432</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>489</v>
+        <v>433</v>
       </c>
     </row>
     <row r="9" spans="1:1">
@@ -13220,12 +13244,12 @@
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>490</v>
+        <v>434</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>491</v>
+        <v>435</v>
       </c>
     </row>
     <row r="14" spans="1:1">
@@ -13245,12 +13269,12 @@
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>492</v>
+        <v>436</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>493</v>
+        <v>437</v>
       </c>
     </row>
     <row r="19" spans="1:1">
@@ -13270,12 +13294,12 @@
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>378</v>
+        <v>350</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>379</v>
+        <v>351</v>
       </c>
     </row>
     <row r="24" spans="1:1">
@@ -13295,12 +13319,12 @@
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>380</v>
+        <v>352</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>381</v>
+        <v>353</v>
       </c>
     </row>
     <row r="29" spans="1:1">
@@ -13320,12 +13344,12 @@
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>382</v>
+        <v>354</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>383</v>
+        <v>355</v>
       </c>
     </row>
     <row r="34" spans="1:1">
@@ -13345,12 +13369,12 @@
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>494</v>
+        <v>438</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>495</v>
+        <v>439</v>
       </c>
     </row>
     <row r="39" spans="1:1">
@@ -13365,12 +13389,12 @@
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>496</v>
+        <v>440</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>497</v>
+        <v>441</v>
       </c>
     </row>
     <row r="44" spans="1:1">
@@ -13385,12 +13409,12 @@
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>498</v>
+        <v>442</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>499</v>
+        <v>443</v>
       </c>
     </row>
     <row r="49" spans="1:1">
@@ -13405,12 +13429,12 @@
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="s">
-        <v>500</v>
+        <v>444</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>501</v>
+        <v>445</v>
       </c>
     </row>
     <row r="54" spans="1:1">
@@ -13430,12 +13454,12 @@
     </row>
     <row r="57" spans="1:1">
       <c r="A57" t="s">
-        <v>384</v>
+        <v>356</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" t="s">
-        <v>385</v>
+        <v>357</v>
       </c>
     </row>
     <row r="59" spans="1:1">
@@ -13455,12 +13479,12 @@
     </row>
     <row r="62" spans="1:1">
       <c r="A62" t="s">
-        <v>386</v>
+        <v>358</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" t="s">
-        <v>387</v>
+        <v>359</v>
       </c>
     </row>
     <row r="64" spans="1:1">
@@ -13480,12 +13504,12 @@
     </row>
     <row r="67" spans="1:1">
       <c r="A67" t="s">
-        <v>388</v>
+        <v>360</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" t="s">
-        <v>389</v>
+        <v>361</v>
       </c>
     </row>
     <row r="69" spans="1:1">
@@ -13505,12 +13529,12 @@
     </row>
     <row r="72" spans="1:1">
       <c r="A72" t="s">
-        <v>502</v>
+        <v>446</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" t="s">
-        <v>503</v>
+        <v>447</v>
       </c>
     </row>
     <row r="74" spans="1:1">
@@ -13525,12 +13549,12 @@
     </row>
     <row r="77" spans="1:1">
       <c r="A77" t="s">
-        <v>504</v>
+        <v>448</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" t="s">
-        <v>505</v>
+        <v>449</v>
       </c>
     </row>
     <row r="79" spans="1:1">
@@ -13545,12 +13569,12 @@
     </row>
     <row r="82" spans="1:1">
       <c r="A82" t="s">
-        <v>506</v>
+        <v>450</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" t="s">
-        <v>507</v>
+        <v>451</v>
       </c>
     </row>
     <row r="84" spans="1:1">
@@ -13565,12 +13589,12 @@
     </row>
     <row r="87" spans="1:1">
       <c r="A87" t="s">
-        <v>508</v>
+        <v>452</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" t="s">
-        <v>509</v>
+        <v>453</v>
       </c>
     </row>
     <row r="89" spans="1:1">
@@ -13590,17 +13614,17 @@
     </row>
     <row r="92" spans="1:1">
       <c r="A92" t="s">
-        <v>390</v>
+        <v>510</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" t="s">
-        <v>391</v>
+        <v>511</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="96" spans="1:1">
@@ -13610,17 +13634,17 @@
     </row>
     <row r="97" spans="1:1">
       <c r="A97" t="s">
-        <v>392</v>
+        <v>512</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" t="s">
-        <v>393</v>
+        <v>513</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="101" spans="1:1">
@@ -13630,17 +13654,17 @@
     </row>
     <row r="102" spans="1:1">
       <c r="A102" t="s">
-        <v>394</v>
+        <v>514</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" t="s">
-        <v>395</v>
+        <v>515</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
     </row>
     <row r="105" spans="1:1">
@@ -13655,17 +13679,17 @@
     </row>
     <row r="107" spans="1:1">
       <c r="A107" t="s">
-        <v>510</v>
+        <v>454</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108" t="s">
-        <v>511</v>
+        <v>455</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="111" spans="1:1">
@@ -13675,17 +13699,17 @@
     </row>
     <row r="112" spans="1:1">
       <c r="A112" t="s">
-        <v>512</v>
+        <v>456</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" t="s">
-        <v>513</v>
+        <v>457</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
     </row>
     <row r="116" spans="1:1">
@@ -13695,17 +13719,17 @@
     </row>
     <row r="117" spans="1:1">
       <c r="A117" t="s">
-        <v>514</v>
+        <v>458</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" t="s">
-        <v>515</v>
+        <v>459</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
     </row>
     <row r="121" spans="1:1">
@@ -13715,17 +13739,17 @@
     </row>
     <row r="122" spans="1:1">
       <c r="A122" t="s">
-        <v>516</v>
+        <v>460</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" t="s">
-        <v>517</v>
+        <v>461</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
     </row>
     <row r="125" spans="1:1">
@@ -13740,17 +13764,17 @@
     </row>
     <row r="127" spans="1:1">
       <c r="A127" t="s">
-        <v>396</v>
+        <v>516</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128" t="s">
-        <v>397</v>
+        <v>517</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
     </row>
     <row r="131" spans="1:1">
@@ -13760,17 +13784,17 @@
     </row>
     <row r="132" spans="1:1">
       <c r="A132" t="s">
-        <v>398</v>
+        <v>518</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133" t="s">
-        <v>399</v>
+        <v>519</v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
     </row>
     <row r="136" spans="1:1">
@@ -13780,17 +13804,17 @@
     </row>
     <row r="137" spans="1:1">
       <c r="A137" t="s">
-        <v>400</v>
+        <v>520</v>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138" t="s">
-        <v>401</v>
+        <v>521</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139" t="s">
-        <v>319</v>
+        <v>307</v>
       </c>
     </row>
     <row r="140" spans="1:1">
@@ -13805,17 +13829,17 @@
     </row>
     <row r="142" spans="1:1">
       <c r="A142" t="s">
-        <v>518</v>
+        <v>462</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143" t="s">
-        <v>519</v>
+        <v>463</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144" t="s">
-        <v>320</v>
+        <v>308</v>
       </c>
     </row>
     <row r="146" spans="1:1">
@@ -13825,17 +13849,17 @@
     </row>
     <row r="147" spans="1:1">
       <c r="A147" t="s">
-        <v>520</v>
+        <v>464</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148" t="s">
-        <v>521</v>
+        <v>465</v>
       </c>
     </row>
     <row r="149" spans="1:1">
       <c r="A149" t="s">
-        <v>321</v>
+        <v>309</v>
       </c>
     </row>
     <row r="151" spans="1:1">
@@ -13845,17 +13869,17 @@
     </row>
     <row r="152" spans="1:1">
       <c r="A152" t="s">
-        <v>522</v>
+        <v>466</v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153" t="s">
-        <v>523</v>
+        <v>467</v>
       </c>
     </row>
     <row r="154" spans="1:1">
       <c r="A154" t="s">
-        <v>322</v>
+        <v>310</v>
       </c>
     </row>
     <row r="156" spans="1:1">
@@ -13865,17 +13889,17 @@
     </row>
     <row r="157" spans="1:1">
       <c r="A157" t="s">
-        <v>524</v>
+        <v>468</v>
       </c>
     </row>
     <row r="158" spans="1:1">
       <c r="A158" t="s">
-        <v>525</v>
+        <v>469</v>
       </c>
     </row>
     <row r="159" spans="1:1">
       <c r="A159" t="s">
-        <v>323</v>
+        <v>311</v>
       </c>
     </row>
     <row r="161" spans="1:1">
@@ -13885,17 +13909,17 @@
     </row>
     <row r="162" spans="1:1">
       <c r="A162" t="s">
-        <v>526</v>
+        <v>470</v>
       </c>
     </row>
     <row r="163" spans="1:1">
       <c r="A163" t="s">
-        <v>527</v>
+        <v>471</v>
       </c>
     </row>
     <row r="164" spans="1:1">
       <c r="A164" t="s">
-        <v>324</v>
+        <v>312</v>
       </c>
     </row>
     <row r="166" spans="1:1">
@@ -13905,17 +13929,17 @@
     </row>
     <row r="167" spans="1:1">
       <c r="A167" t="s">
-        <v>528</v>
+        <v>472</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168" t="s">
-        <v>529</v>
+        <v>473</v>
       </c>
     </row>
     <row r="169" spans="1:1">
       <c r="A169" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
     </row>
     <row r="171" spans="1:1">
@@ -13925,17 +13949,17 @@
     </row>
     <row r="172" spans="1:1">
       <c r="A172" t="s">
-        <v>530</v>
+        <v>474</v>
       </c>
     </row>
     <row r="173" spans="1:1">
       <c r="A173" t="s">
-        <v>531</v>
+        <v>475</v>
       </c>
     </row>
     <row r="174" spans="1:1">
       <c r="A174" t="s">
-        <v>326</v>
+        <v>314</v>
       </c>
     </row>
     <row r="176" spans="1:1">
@@ -13945,17 +13969,17 @@
     </row>
     <row r="177" spans="1:1">
       <c r="A177" t="s">
-        <v>532</v>
+        <v>476</v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178" t="s">
-        <v>533</v>
+        <v>477</v>
       </c>
     </row>
     <row r="179" spans="1:1">
       <c r="A179" t="s">
-        <v>327</v>
+        <v>315</v>
       </c>
     </row>
     <row r="181" spans="1:1">
@@ -13965,17 +13989,17 @@
     </row>
     <row r="182" spans="1:1">
       <c r="A182" t="s">
-        <v>534</v>
+        <v>478</v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183" t="s">
-        <v>535</v>
+        <v>479</v>
       </c>
     </row>
     <row r="184" spans="1:1">
       <c r="A184" t="s">
-        <v>328</v>
+        <v>316</v>
       </c>
     </row>
     <row r="186" spans="1:1">
@@ -13985,17 +14009,17 @@
     </row>
     <row r="187" spans="1:1">
       <c r="A187" t="s">
-        <v>536</v>
+        <v>480</v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188" t="s">
-        <v>537</v>
+        <v>481</v>
       </c>
     </row>
     <row r="189" spans="1:1">
       <c r="A189" t="s">
-        <v>329</v>
+        <v>317</v>
       </c>
     </row>
     <row r="190" spans="1:1">
@@ -14010,17 +14034,17 @@
     </row>
     <row r="192" spans="1:1">
       <c r="A192" t="s">
-        <v>402</v>
+        <v>522</v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193" t="s">
-        <v>403</v>
+        <v>523</v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194" t="s">
-        <v>332</v>
+        <v>318</v>
       </c>
     </row>
     <row r="196" spans="1:1">
@@ -14030,17 +14054,17 @@
     </row>
     <row r="197" spans="1:1">
       <c r="A197" t="s">
-        <v>404</v>
+        <v>524</v>
       </c>
     </row>
     <row r="198" spans="1:1">
       <c r="A198" t="s">
-        <v>405</v>
+        <v>525</v>
       </c>
     </row>
     <row r="199" spans="1:1">
       <c r="A199" t="s">
-        <v>335</v>
+        <v>319</v>
       </c>
     </row>
     <row r="201" spans="1:1">
@@ -14050,17 +14074,17 @@
     </row>
     <row r="202" spans="1:1">
       <c r="A202" t="s">
-        <v>406</v>
+        <v>526</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203" t="s">
-        <v>407</v>
+        <v>527</v>
       </c>
     </row>
     <row r="204" spans="1:1">
       <c r="A204" t="s">
-        <v>338</v>
+        <v>320</v>
       </c>
     </row>
     <row r="206" spans="1:1">
@@ -14070,17 +14094,17 @@
     </row>
     <row r="207" spans="1:1">
       <c r="A207" t="s">
-        <v>408</v>
+        <v>528</v>
       </c>
     </row>
     <row r="208" spans="1:1">
       <c r="A208" t="s">
-        <v>409</v>
+        <v>529</v>
       </c>
     </row>
     <row r="209" spans="1:1">
       <c r="A209" t="s">
-        <v>341</v>
+        <v>321</v>
       </c>
     </row>
     <row r="211" spans="1:1">
@@ -14090,17 +14114,17 @@
     </row>
     <row r="212" spans="1:1">
       <c r="A212" t="s">
-        <v>410</v>
+        <v>530</v>
       </c>
     </row>
     <row r="213" spans="1:1">
       <c r="A213" t="s">
-        <v>411</v>
+        <v>531</v>
       </c>
     </row>
     <row r="214" spans="1:1">
       <c r="A214" t="s">
-        <v>344</v>
+        <v>322</v>
       </c>
     </row>
     <row r="216" spans="1:1">
@@ -14110,17 +14134,17 @@
     </row>
     <row r="217" spans="1:1">
       <c r="A217" t="s">
-        <v>412</v>
+        <v>532</v>
       </c>
     </row>
     <row r="218" spans="1:1">
       <c r="A218" t="s">
-        <v>413</v>
+        <v>533</v>
       </c>
     </row>
     <row r="219" spans="1:1">
       <c r="A219" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
     </row>
     <row r="221" spans="1:1">
@@ -14130,17 +14154,17 @@
     </row>
     <row r="222" spans="1:1">
       <c r="A222" t="s">
-        <v>414</v>
+        <v>534</v>
       </c>
     </row>
     <row r="223" spans="1:1">
       <c r="A223" t="s">
-        <v>415</v>
+        <v>535</v>
       </c>
     </row>
     <row r="224" spans="1:1">
       <c r="A224" t="s">
-        <v>350</v>
+        <v>324</v>
       </c>
     </row>
     <row r="226" spans="1:1">
@@ -14150,17 +14174,17 @@
     </row>
     <row r="227" spans="1:1">
       <c r="A227" t="s">
-        <v>416</v>
+        <v>536</v>
       </c>
     </row>
     <row r="228" spans="1:1">
       <c r="A228" t="s">
-        <v>417</v>
+        <v>537</v>
       </c>
     </row>
     <row r="229" spans="1:1">
       <c r="A229" t="s">
-        <v>353</v>
+        <v>325</v>
       </c>
     </row>
     <row r="230" spans="1:1">
@@ -14175,17 +14199,17 @@
     </row>
     <row r="232" spans="1:1">
       <c r="A232" t="s">
-        <v>418</v>
+        <v>362</v>
       </c>
     </row>
     <row r="233" spans="1:1">
       <c r="A233" t="s">
-        <v>419</v>
+        <v>363</v>
       </c>
     </row>
     <row r="234" spans="1:1">
       <c r="A234" t="s">
-        <v>356</v>
+        <v>328</v>
       </c>
     </row>
     <row r="235" spans="1:1">
@@ -14200,17 +14224,17 @@
     </row>
     <row r="237" spans="1:1">
       <c r="A237" t="s">
-        <v>420</v>
+        <v>364</v>
       </c>
     </row>
     <row r="238" spans="1:1">
       <c r="A238" t="s">
-        <v>421</v>
+        <v>365</v>
       </c>
     </row>
     <row r="239" spans="1:1">
       <c r="A239" t="s">
-        <v>359</v>
+        <v>331</v>
       </c>
     </row>
     <row r="240" spans="1:1">
@@ -14225,17 +14249,17 @@
     </row>
     <row r="242" spans="1:1">
       <c r="A242" t="s">
-        <v>422</v>
+        <v>366</v>
       </c>
     </row>
     <row r="243" spans="1:1">
       <c r="A243" t="s">
-        <v>423</v>
+        <v>367</v>
       </c>
     </row>
     <row r="244" spans="1:1">
       <c r="A244" t="s">
-        <v>362</v>
+        <v>334</v>
       </c>
     </row>
     <row r="245" spans="1:1">
@@ -14250,17 +14274,17 @@
     </row>
     <row r="247" spans="1:1">
       <c r="A247" t="s">
-        <v>424</v>
+        <v>368</v>
       </c>
     </row>
     <row r="248" spans="1:1">
       <c r="A248" t="s">
-        <v>425</v>
+        <v>369</v>
       </c>
     </row>
     <row r="249" spans="1:1">
       <c r="A249" t="s">
-        <v>365</v>
+        <v>337</v>
       </c>
     </row>
     <row r="250" spans="1:1">
@@ -14275,17 +14299,17 @@
     </row>
     <row r="252" spans="1:1">
       <c r="A252" t="s">
-        <v>426</v>
+        <v>370</v>
       </c>
     </row>
     <row r="253" spans="1:1">
       <c r="A253" t="s">
-        <v>427</v>
+        <v>371</v>
       </c>
     </row>
     <row r="254" spans="1:1">
       <c r="A254" t="s">
-        <v>368</v>
+        <v>340</v>
       </c>
     </row>
     <row r="255" spans="1:1">
@@ -14300,17 +14324,17 @@
     </row>
     <row r="257" spans="1:1">
       <c r="A257" t="s">
-        <v>428</v>
+        <v>372</v>
       </c>
     </row>
     <row r="258" spans="1:1">
       <c r="A258" t="s">
-        <v>429</v>
+        <v>373</v>
       </c>
     </row>
     <row r="259" spans="1:1">
       <c r="A259" t="s">
-        <v>371</v>
+        <v>343</v>
       </c>
     </row>
     <row r="260" spans="1:1">
@@ -14325,17 +14349,17 @@
     </row>
     <row r="262" spans="1:1">
       <c r="A262" t="s">
-        <v>430</v>
+        <v>374</v>
       </c>
     </row>
     <row r="263" spans="1:1">
       <c r="A263" t="s">
-        <v>431</v>
+        <v>375</v>
       </c>
     </row>
     <row r="264" spans="1:1">
       <c r="A264" t="s">
-        <v>374</v>
+        <v>346</v>
       </c>
     </row>
     <row r="265" spans="1:1">
@@ -14350,17 +14374,17 @@
     </row>
     <row r="267" spans="1:1">
       <c r="A267" t="s">
-        <v>432</v>
+        <v>376</v>
       </c>
     </row>
     <row r="268" spans="1:1">
       <c r="A268" t="s">
-        <v>433</v>
+        <v>377</v>
       </c>
     </row>
     <row r="269" spans="1:1">
       <c r="A269" t="s">
-        <v>377</v>
+        <v>349</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added 10000 perm test, renamed commands files to reflect number of perms
</commit_message>
<xml_diff>
--- a/datasets/AMETHST_data/amethst_commands.xlsx
+++ b/datasets/AMETHST_data/amethst_commands.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="-20" windowWidth="38400" windowHeight="21180" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="amethst_commands" sheetId="1" r:id="rId1"/>
-    <sheet name="full commands text" sheetId="2" r:id="rId2"/>
-    <sheet name="test commands text" sheetId="3" r:id="rId3"/>
+    <sheet name="10_perm" sheetId="3" r:id="rId2"/>
+    <sheet name="1,000_perm" sheetId="2" r:id="rId3"/>
+    <sheet name="10,000_perm" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3242" uniqueCount="541">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3482" uniqueCount="649">
   <si>
     <t>#job</t>
   </si>
@@ -1644,6 +1645,330 @@
   </si>
   <si>
     <t>plot_pco_with_stats_all.pl --data_file 10.Qiime.Qiime_default.removed.norm --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree 97_otus.tree --num_cpus 10 --output_prefix Analysis_54b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 4.MG-RAST.MG-RAST_default.included.norm --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method bray-curtis --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_1w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 4.MG-RAST.MG-RAST_default.included.norm --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method bray-curtis --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_1b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 3.MG-RAST.MG-RAST_default.included.raw --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method bray-curtis --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_2w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 3.MG-RAST.MG-RAST_default.included.raw --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method bray-curtis --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_2b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 4.MG-RAST.MG-RAST_default.included.norm --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_3w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 4.MG-RAST.MG-RAST_default.included.norm --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_3b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 3.MG-RAST.MG-RAST_default.included.raw --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_4w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 3.MG-RAST.MG-RAST_default.included.raw --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_4b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 11.Qiime.Qiime_default.included.raw --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree 97_otus.tree --num_cpus 10 --output_prefix Analysis_5w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 11.Qiime.Qiime_default.included.raw --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree 97_otus.tree --num_cpus 10 --output_prefix Analysis_5b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 12.Qiime.Qiime_default.included.norm --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree 97_otus.tree --num_cpus 10 --output_prefix Analysis_6w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 12.Qiime.Qiime_default.included.norm --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree 97_otus.tree --num_cpus 10 --output_prefix Analysis_6b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 11.Qiime.Qiime_default.included.raw --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree 97_otus.tree --num_cpus 10 --output_prefix Analysis_7w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 11.Qiime.Qiime_default.included.raw --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree 97_otus.tree --num_cpus 10 --output_prefix Analysis_7b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 2.MG-RAST.MG-RAST_default.removed.norm --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method bray-curtis --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_8w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 2.MG-RAST.MG-RAST_default.removed.norm --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method bray-curtis --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_8b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 1.MG-RAST.MG-RAST_default.removed.raw --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method bray-curtis --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_9w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 1.MG-RAST.MG-RAST_default.removed.raw --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method bray-curtis --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_9b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 2.MG-RAST.MG-RAST_default.removed.norm --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_10w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 2.MG-RAST.MG-RAST_default.removed.norm --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_10b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 1.MG-RAST.MG-RAST_default.removed.raw --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_11w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 1.MG-RAST.MG-RAST_default.removed.raw --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_11b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 9.Qiime.Qiime_default.removed.raw --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree 97_otus.tree --num_cpus 10 --output_prefix Analysis_12w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 9.Qiime.Qiime_default.removed.raw --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree 97_otus.tree --num_cpus 10 --output_prefix Analysis_12b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 10.Qiime.Qiime_default.removed.norm --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree 97_otus.tree --num_cpus 10 --output_prefix Analysis_13w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 10.Qiime.Qiime_default.removed.norm --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree 97_otus.tree --num_cpus 10 --output_prefix Analysis_13b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 9.Qiime.Qiime_default.removed.raw --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree 97_otus.tree --num_cpus 10 --output_prefix Analysis_14w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 9.Qiime.Qiime_default.removed.raw --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree 97_otus.tree --num_cpus 10 --output_prefix Analysis_14b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 8.MG-RAST.100p.included.norm --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method bray-curtis --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_15w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 8.MG-RAST.100p.included.norm --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method bray-curtis --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_15b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 7.MG-RAST.100p.included.raw --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method bray-curtis --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_16w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 7.MG-RAST.100p.included.raw --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method bray-curtis --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_16b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 8.MG-RAST.100p.included.norm --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_17w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 8.MG-RAST.100p.included.norm --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_17b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 7.MG-RAST.100p.included.raw --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_18w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 7.MG-RAST.100p.included.raw --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_18b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree 16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_19w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree 16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_19b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 16.Qiime.100p.included.norm --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree 16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_20w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 16.Qiime.100p.included.norm --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree 16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_20b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree 16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_21w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree 16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_21b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 6.MG-RAST.100p.removed.norm --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method bray-curtis --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_22w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 6.MG-RAST.100p.removed.norm --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method bray-curtis --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_22b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 5.MG-RAST.100p.removed.raw --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method bray-curtis --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_23w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 5.MG-RAST.100p.removed.raw --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method bray-curtis --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_23b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 6.MG-RAST.100p.removed.norm --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_24w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 6.MG-RAST.100p.removed.norm --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_24b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 5.MG-RAST.100p.removed.raw --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_25w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 5.MG-RAST.100p.removed.raw --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_25b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree 16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_26w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree 16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_26b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 14.Qiime.100p.removed.norm --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree 16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_27w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 14.Qiime.100p.removed.norm --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree 16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_27b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree 16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_28w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method weighted_unifrac --dist_pipe qiime_pipe --qiime_format qiime_table --tree 16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_28b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 3.MG-RAST.MG-RAST_default.included.raw --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_29w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 3.MG-RAST.MG-RAST_default.included.raw --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_29b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 4.MG-RAST.MG-RAST_default.included.norm --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_30w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 4.MG-RAST.MG-RAST_default.included.norm --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_30b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 7.MG-RAST.100p.included.raw --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_31w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 7.MG-RAST.100p.included.raw --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_31b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 8.MG-RAST.100p.included.norm --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_32w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 8.MG-RAST.100p.included.norm --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_32b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 3.MG-RAST.MG-RAST_default.included.raw --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_33w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 3.MG-RAST.MG-RAST_default.included.raw --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_33b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 4.MG-RAST.MG-RAST_default.included.norm --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_34w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 4.MG-RAST.MG-RAST_default.included.norm --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_34b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 7.MG-RAST.100p.included.raw --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_35w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 7.MG-RAST.100p.included.raw --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_35b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 8.MG-RAST.100p.included.norm --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_36w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 8.MG-RAST.100p.included.norm --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method euclidean --dist_pipe MG-RAST_pipe --num_cpus 10 --output_prefix Analysis_36b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 3.MG-RAST.MG-RAST_default.included.raw --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method OTU --dist_pipe OTU_pipe --num_cpus 10 --output_prefix Analysis_37w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 3.MG-RAST.MG-RAST_default.included.raw --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method OTU --dist_pipe OTU_pipe --num_cpus 10 --output_prefix Analysis_37b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 3.MG-RAST.MG-RAST_default.included.raw --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method w_OTU --dist_pipe OTU_pipe --num_cpus 10 --output_prefix Analysis_38w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 3.MG-RAST.MG-RAST_default.included.raw --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method w_OTU --dist_pipe OTU_pipe --num_cpus 10 --output_prefix Analysis_38b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree 16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_39w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree 16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_39b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 16.Qiime.100p.included.norm --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree 16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_40w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 16.Qiime.100p.included.norm --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree 16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_40b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree 16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_41w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree 16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_41b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 14.Qiime.100p.removed.norm --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree 16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_42w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 14.Qiime.100p.removed.norm --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree 16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_42b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree 16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_43w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 15.Qiime.100p.included.raw --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree 16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_43b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 16.Qiime.100p.included.norm --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree 16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_44w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 16.Qiime.100p.included.norm --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree 16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_44b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree 16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_45w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 13.Qiime.100p.removed.raw --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree 16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_45b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 14.Qiime.100p.removed.norm --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree 16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_46w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 14.Qiime.100p.removed.norm --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree 16S_all_gg_2011_1.tree --num_cpus 10 --output_prefix Analysis_46b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 11.Qiime.Qiime_default.included.raw --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree 97_otus.tree --num_cpus 10 --output_prefix Analysis_47w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 11.Qiime.Qiime_default.included.raw --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree 97_otus.tree --num_cpus 10 --output_prefix Analysis_47b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 11.Qiime.Qiime_default.included.raw --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree 97_otus.tree --num_cpus 10 --output_prefix Analysis_48w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 11.Qiime.Qiime_default.included.raw --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree 97_otus.tree --num_cpus 10 --output_prefix Analysis_48b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 9.Qiime.Qiime_default.removed.raw --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree 97_otus.tree --num_cpus 10 --output_prefix Analysis_49w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 9.Qiime.Qiime_default.removed.raw --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree 97_otus.tree --num_cpus 10 --output_prefix Analysis_49b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 9.Qiime.Qiime_default.removed.raw --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree 97_otus.tree --num_cpus 10 --output_prefix Analysis_50w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 9.Qiime.Qiime_default.removed.raw --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree 97_otus.tree --num_cpus 10 --output_prefix Analysis_50b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 12.Qiime.Qiime_default.included.norm --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree 97_otus.tree --num_cpus 10 --output_prefix Analysis_51w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 12.Qiime.Qiime_default.included.norm --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree 97_otus.tree --num_cpus 10 --output_prefix Analysis_51b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 12.Qiime.Qiime_default.included.norm --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree 97_otus.tree --num_cpus 10 --output_prefix Analysis_52w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 12.Qiime.Qiime_default.included.norm --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree 97_otus.tree --num_cpus 10 --output_prefix Analysis_52b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 10.Qiime.Qiime_default.removed.norm --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree 97_otus.tree --num_cpus 10 --output_prefix Analysis_53w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 10.Qiime.Qiime_default.removed.norm --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method bray_curtis --dist_pipe qiime_pipe --qiime_format qiime_table --tree 97_otus.tree --num_cpus 10 --output_prefix Analysis_53b --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 10.Qiime.Qiime_default.removed.norm --sig_if lt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type dataset_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree 97_otus.tree --num_cpus 10 --output_prefix Analysis_54w --cleanup</t>
+  </si>
+  <si>
+    <t>plot_pco_with_stats_all.pl --data_file 10.Qiime.Qiime_default.removed.norm --sig_if gt --groups_list AMETHST.stat.groups --num_perm 10000 --perm_type rowwise_rand --dist_method euclidean --dist_pipe qiime_pipe --qiime_format qiime_table --tree 97_otus.tree --num_cpus 10 --output_prefix Analysis_54b --cleanup</t>
   </si>
 </sst>
 </file>
@@ -1692,8 +2017,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="179">
+  <cellStyleXfs count="181">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1877,7 +2204,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="179">
+  <cellStyles count="181">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1967,6 +2294,7 @@
     <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2056,6 +2384,7 @@
     <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -12786,10 +13115,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A269"/>
+  <dimension ref="A1:Y269"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:A1048576"/>
+    <sheetView topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="Y77" sqref="Y77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -12801,12 +13130,12 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>323</v>
+        <v>375</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>324</v>
+        <v>376</v>
       </c>
     </row>
     <row r="4" spans="1:1">
@@ -12826,12 +13155,12 @@
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>325</v>
+        <v>377</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>326</v>
+        <v>378</v>
       </c>
     </row>
     <row r="9" spans="1:1">
@@ -12851,12 +13180,12 @@
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>327</v>
+        <v>379</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>328</v>
+        <v>380</v>
       </c>
     </row>
     <row r="14" spans="1:1">
@@ -12876,12 +13205,12 @@
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>329</v>
+        <v>381</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>330</v>
+        <v>382</v>
       </c>
     </row>
     <row r="19" spans="1:1">
@@ -12901,12 +13230,12 @@
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>429</v>
+        <v>485</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>430</v>
+        <v>486</v>
       </c>
     </row>
     <row r="24" spans="1:1">
@@ -12926,12 +13255,12 @@
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>431</v>
+        <v>487</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>432</v>
+        <v>488</v>
       </c>
     </row>
     <row r="29" spans="1:1">
@@ -12951,12 +13280,12 @@
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>433</v>
+        <v>489</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>434</v>
+        <v>490</v>
       </c>
     </row>
     <row r="34" spans="1:1">
@@ -12976,12 +13305,12 @@
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>331</v>
+        <v>383</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>332</v>
+        <v>384</v>
       </c>
     </row>
     <row r="39" spans="1:1">
@@ -12996,12 +13325,12 @@
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>333</v>
+        <v>385</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>334</v>
+        <v>386</v>
       </c>
     </row>
     <row r="44" spans="1:1">
@@ -13016,12 +13345,12 @@
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>335</v>
+        <v>387</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>336</v>
+        <v>388</v>
       </c>
     </row>
     <row r="49" spans="1:1">
@@ -13036,12 +13365,12 @@
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="s">
-        <v>337</v>
+        <v>389</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>338</v>
+        <v>390</v>
       </c>
     </row>
     <row r="54" spans="1:1">
@@ -13061,12 +13390,12 @@
     </row>
     <row r="57" spans="1:1">
       <c r="A57" t="s">
-        <v>435</v>
+        <v>491</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" t="s">
-        <v>436</v>
+        <v>492</v>
       </c>
     </row>
     <row r="59" spans="1:1">
@@ -13086,12 +13415,12 @@
     </row>
     <row r="62" spans="1:1">
       <c r="A62" t="s">
-        <v>437</v>
+        <v>493</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" t="s">
-        <v>438</v>
+        <v>494</v>
       </c>
     </row>
     <row r="64" spans="1:1">
@@ -13099,72 +13428,76 @@
         <v>278</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:25">
       <c r="A65" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:25">
       <c r="A66" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:25">
       <c r="A67" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="68" spans="1:25">
       <c r="A68" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="69" spans="1:25">
       <c r="A69" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:25">
       <c r="A70" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:25">
       <c r="A71" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:25">
       <c r="A72" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="73" spans="1:25">
       <c r="A73" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="74" spans="1:25">
       <c r="A74" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="76" spans="1:1">
+    <row r="76" spans="1:25">
       <c r="A76" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="77" spans="1:1">
+    <row r="77" spans="1:25">
       <c r="A77" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1">
+        <v>393</v>
+      </c>
+      <c r="Y77">
+        <f>0.0002/0.000001</f>
+        <v>200.00000000000003</v>
+      </c>
+    </row>
+    <row r="78" spans="1:25">
       <c r="A78" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="79" spans="1:25">
       <c r="A79" t="s">
         <v>281</v>
       </c>
@@ -13176,12 +13509,12 @@
     </row>
     <row r="82" spans="1:1">
       <c r="A82" t="s">
-        <v>343</v>
+        <v>395</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" t="s">
-        <v>344</v>
+        <v>396</v>
       </c>
     </row>
     <row r="84" spans="1:1">
@@ -13196,12 +13529,12 @@
     </row>
     <row r="87" spans="1:1">
       <c r="A87" t="s">
-        <v>345</v>
+        <v>397</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" t="s">
-        <v>346</v>
+        <v>398</v>
       </c>
     </row>
     <row r="89" spans="1:1">
@@ -13221,12 +13554,12 @@
     </row>
     <row r="92" spans="1:1">
       <c r="A92" t="s">
-        <v>441</v>
+        <v>497</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" t="s">
-        <v>442</v>
+        <v>498</v>
       </c>
     </row>
     <row r="94" spans="1:1">
@@ -13241,12 +13574,12 @@
     </row>
     <row r="97" spans="1:1">
       <c r="A97" t="s">
-        <v>443</v>
+        <v>499</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" t="s">
-        <v>444</v>
+        <v>500</v>
       </c>
     </row>
     <row r="99" spans="1:1">
@@ -13261,12 +13594,12 @@
     </row>
     <row r="102" spans="1:1">
       <c r="A102" t="s">
-        <v>445</v>
+        <v>501</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" t="s">
-        <v>446</v>
+        <v>502</v>
       </c>
     </row>
     <row r="104" spans="1:1">
@@ -13286,12 +13619,12 @@
     </row>
     <row r="107" spans="1:1">
       <c r="A107" t="s">
-        <v>347</v>
+        <v>399</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108" t="s">
-        <v>348</v>
+        <v>400</v>
       </c>
     </row>
     <row r="109" spans="1:1">
@@ -13306,12 +13639,12 @@
     </row>
     <row r="112" spans="1:1">
       <c r="A112" t="s">
-        <v>349</v>
+        <v>401</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" t="s">
-        <v>350</v>
+        <v>402</v>
       </c>
     </row>
     <row r="114" spans="1:1">
@@ -13326,12 +13659,12 @@
     </row>
     <row r="117" spans="1:1">
       <c r="A117" t="s">
-        <v>351</v>
+        <v>403</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" t="s">
-        <v>352</v>
+        <v>404</v>
       </c>
     </row>
     <row r="119" spans="1:1">
@@ -13346,12 +13679,12 @@
     </row>
     <row r="122" spans="1:1">
       <c r="A122" t="s">
-        <v>353</v>
+        <v>405</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" t="s">
-        <v>354</v>
+        <v>406</v>
       </c>
     </row>
     <row r="124" spans="1:1">
@@ -13371,12 +13704,12 @@
     </row>
     <row r="127" spans="1:1">
       <c r="A127" t="s">
-        <v>447</v>
+        <v>503</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128" t="s">
-        <v>448</v>
+        <v>504</v>
       </c>
     </row>
     <row r="129" spans="1:1">
@@ -13391,12 +13724,12 @@
     </row>
     <row r="132" spans="1:1">
       <c r="A132" t="s">
-        <v>449</v>
+        <v>505</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133" t="s">
-        <v>450</v>
+        <v>506</v>
       </c>
     </row>
     <row r="134" spans="1:1">
@@ -13411,12 +13744,12 @@
     </row>
     <row r="137" spans="1:1">
       <c r="A137" t="s">
-        <v>451</v>
+        <v>507</v>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138" t="s">
-        <v>452</v>
+        <v>508</v>
       </c>
     </row>
     <row r="139" spans="1:1">
@@ -13436,12 +13769,12 @@
     </row>
     <row r="142" spans="1:1">
       <c r="A142" t="s">
-        <v>355</v>
+        <v>407</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143" t="s">
-        <v>356</v>
+        <v>408</v>
       </c>
     </row>
     <row r="144" spans="1:1">
@@ -13456,12 +13789,12 @@
     </row>
     <row r="147" spans="1:1">
       <c r="A147" t="s">
-        <v>357</v>
+        <v>409</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148" t="s">
-        <v>358</v>
+        <v>410</v>
       </c>
     </row>
     <row r="149" spans="1:1">
@@ -13476,12 +13809,12 @@
     </row>
     <row r="152" spans="1:1">
       <c r="A152" t="s">
-        <v>359</v>
+        <v>411</v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153" t="s">
-        <v>360</v>
+        <v>412</v>
       </c>
     </row>
     <row r="154" spans="1:1">
@@ -13496,12 +13829,12 @@
     </row>
     <row r="157" spans="1:1">
       <c r="A157" t="s">
-        <v>361</v>
+        <v>413</v>
       </c>
     </row>
     <row r="158" spans="1:1">
       <c r="A158" t="s">
-        <v>362</v>
+        <v>414</v>
       </c>
     </row>
     <row r="159" spans="1:1">
@@ -13516,12 +13849,12 @@
     </row>
     <row r="162" spans="1:1">
       <c r="A162" t="s">
-        <v>363</v>
+        <v>415</v>
       </c>
     </row>
     <row r="163" spans="1:1">
       <c r="A163" t="s">
-        <v>364</v>
+        <v>416</v>
       </c>
     </row>
     <row r="164" spans="1:1">
@@ -13536,12 +13869,12 @@
     </row>
     <row r="167" spans="1:1">
       <c r="A167" t="s">
-        <v>365</v>
+        <v>417</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168" t="s">
-        <v>366</v>
+        <v>418</v>
       </c>
     </row>
     <row r="169" spans="1:1">
@@ -13556,12 +13889,12 @@
     </row>
     <row r="172" spans="1:1">
       <c r="A172" t="s">
-        <v>367</v>
+        <v>419</v>
       </c>
     </row>
     <row r="173" spans="1:1">
       <c r="A173" t="s">
-        <v>368</v>
+        <v>420</v>
       </c>
     </row>
     <row r="174" spans="1:1">
@@ -13576,12 +13909,12 @@
     </row>
     <row r="177" spans="1:1">
       <c r="A177" t="s">
-        <v>369</v>
+        <v>421</v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178" t="s">
-        <v>370</v>
+        <v>422</v>
       </c>
     </row>
     <row r="179" spans="1:1">
@@ -13596,12 +13929,12 @@
     </row>
     <row r="182" spans="1:1">
       <c r="A182" t="s">
-        <v>371</v>
+        <v>423</v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183" t="s">
-        <v>372</v>
+        <v>424</v>
       </c>
     </row>
     <row r="184" spans="1:1">
@@ -13616,12 +13949,12 @@
     </row>
     <row r="187" spans="1:1">
       <c r="A187" t="s">
-        <v>373</v>
+        <v>425</v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188" t="s">
-        <v>374</v>
+        <v>426</v>
       </c>
     </row>
     <row r="189" spans="1:1">
@@ -13641,12 +13974,12 @@
     </row>
     <row r="192" spans="1:1">
       <c r="A192" t="s">
-        <v>453</v>
+        <v>509</v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193" t="s">
-        <v>454</v>
+        <v>510</v>
       </c>
     </row>
     <row r="194" spans="1:1">
@@ -13661,12 +13994,12 @@
     </row>
     <row r="197" spans="1:1">
       <c r="A197" t="s">
-        <v>455</v>
+        <v>511</v>
       </c>
     </row>
     <row r="198" spans="1:1">
       <c r="A198" t="s">
-        <v>456</v>
+        <v>512</v>
       </c>
     </row>
     <row r="199" spans="1:1">
@@ -13681,12 +14014,12 @@
     </row>
     <row r="202" spans="1:1">
       <c r="A202" t="s">
-        <v>457</v>
+        <v>513</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203" t="s">
-        <v>458</v>
+        <v>514</v>
       </c>
     </row>
     <row r="204" spans="1:1">
@@ -13701,12 +14034,12 @@
     </row>
     <row r="207" spans="1:1">
       <c r="A207" t="s">
-        <v>459</v>
+        <v>515</v>
       </c>
     </row>
     <row r="208" spans="1:1">
       <c r="A208" t="s">
-        <v>460</v>
+        <v>516</v>
       </c>
     </row>
     <row r="209" spans="1:1">
@@ -13721,12 +14054,12 @@
     </row>
     <row r="212" spans="1:1">
       <c r="A212" t="s">
-        <v>461</v>
+        <v>517</v>
       </c>
     </row>
     <row r="213" spans="1:1">
       <c r="A213" t="s">
-        <v>462</v>
+        <v>518</v>
       </c>
     </row>
     <row r="214" spans="1:1">
@@ -13741,12 +14074,12 @@
     </row>
     <row r="217" spans="1:1">
       <c r="A217" t="s">
-        <v>463</v>
+        <v>519</v>
       </c>
     </row>
     <row r="218" spans="1:1">
       <c r="A218" t="s">
-        <v>464</v>
+        <v>520</v>
       </c>
     </row>
     <row r="219" spans="1:1">
@@ -13761,12 +14094,12 @@
     </row>
     <row r="222" spans="1:1">
       <c r="A222" t="s">
-        <v>465</v>
+        <v>521</v>
       </c>
     </row>
     <row r="223" spans="1:1">
       <c r="A223" t="s">
-        <v>466</v>
+        <v>522</v>
       </c>
     </row>
     <row r="224" spans="1:1">
@@ -13781,12 +14114,12 @@
     </row>
     <row r="227" spans="1:1">
       <c r="A227" t="s">
-        <v>467</v>
+        <v>523</v>
       </c>
     </row>
     <row r="228" spans="1:1">
       <c r="A228" t="s">
-        <v>468</v>
+        <v>524</v>
       </c>
     </row>
     <row r="229" spans="1:1">
@@ -13806,12 +14139,12 @@
     </row>
     <row r="232" spans="1:1">
       <c r="A232" t="s">
-        <v>469</v>
+        <v>525</v>
       </c>
     </row>
     <row r="233" spans="1:1">
       <c r="A233" t="s">
-        <v>470</v>
+        <v>526</v>
       </c>
     </row>
     <row r="234" spans="1:1">
@@ -13831,12 +14164,12 @@
     </row>
     <row r="237" spans="1:1">
       <c r="A237" t="s">
-        <v>471</v>
+        <v>527</v>
       </c>
     </row>
     <row r="238" spans="1:1">
       <c r="A238" t="s">
-        <v>472</v>
+        <v>528</v>
       </c>
     </row>
     <row r="239" spans="1:1">
@@ -13856,12 +14189,12 @@
     </row>
     <row r="242" spans="1:1">
       <c r="A242" t="s">
-        <v>473</v>
+        <v>529</v>
       </c>
     </row>
     <row r="243" spans="1:1">
       <c r="A243" t="s">
-        <v>474</v>
+        <v>530</v>
       </c>
     </row>
     <row r="244" spans="1:1">
@@ -13881,12 +14214,12 @@
     </row>
     <row r="247" spans="1:1">
       <c r="A247" t="s">
-        <v>475</v>
+        <v>531</v>
       </c>
     </row>
     <row r="248" spans="1:1">
       <c r="A248" t="s">
-        <v>476</v>
+        <v>532</v>
       </c>
     </row>
     <row r="249" spans="1:1">
@@ -13906,12 +14239,12 @@
     </row>
     <row r="252" spans="1:1">
       <c r="A252" t="s">
-        <v>477</v>
+        <v>533</v>
       </c>
     </row>
     <row r="253" spans="1:1">
       <c r="A253" t="s">
-        <v>478</v>
+        <v>534</v>
       </c>
     </row>
     <row r="254" spans="1:1">
@@ -13931,12 +14264,12 @@
     </row>
     <row r="257" spans="1:1">
       <c r="A257" t="s">
-        <v>479</v>
+        <v>535</v>
       </c>
     </row>
     <row r="258" spans="1:1">
       <c r="A258" t="s">
-        <v>480</v>
+        <v>536</v>
       </c>
     </row>
     <row r="259" spans="1:1">
@@ -13956,12 +14289,12 @@
     </row>
     <row r="262" spans="1:1">
       <c r="A262" t="s">
-        <v>481</v>
+        <v>537</v>
       </c>
     </row>
     <row r="263" spans="1:1">
       <c r="A263" t="s">
-        <v>482</v>
+        <v>538</v>
       </c>
     </row>
     <row r="264" spans="1:1">
@@ -13981,12 +14314,12 @@
     </row>
     <row r="267" spans="1:1">
       <c r="A267" t="s">
-        <v>483</v>
+        <v>539</v>
       </c>
     </row>
     <row r="268" spans="1:1">
       <c r="A268" t="s">
-        <v>484</v>
+        <v>540</v>
       </c>
     </row>
     <row r="269" spans="1:1">
@@ -14009,8 +14342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A269"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="A97" sqref="A97"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -14022,12 +14355,12 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>375</v>
+        <v>323</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>376</v>
+        <v>324</v>
       </c>
     </row>
     <row r="4" spans="1:1">
@@ -14047,12 +14380,12 @@
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>377</v>
+        <v>325</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>378</v>
+        <v>326</v>
       </c>
     </row>
     <row r="9" spans="1:1">
@@ -14072,12 +14405,12 @@
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>379</v>
+        <v>327</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>380</v>
+        <v>328</v>
       </c>
     </row>
     <row r="14" spans="1:1">
@@ -14097,12 +14430,12 @@
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>381</v>
+        <v>329</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>382</v>
+        <v>330</v>
       </c>
     </row>
     <row r="19" spans="1:1">
@@ -14122,12 +14455,12 @@
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>485</v>
+        <v>429</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>486</v>
+        <v>430</v>
       </c>
     </row>
     <row r="24" spans="1:1">
@@ -14147,12 +14480,12 @@
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>487</v>
+        <v>431</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>488</v>
+        <v>432</v>
       </c>
     </row>
     <row r="29" spans="1:1">
@@ -14172,12 +14505,12 @@
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>489</v>
+        <v>433</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>490</v>
+        <v>434</v>
       </c>
     </row>
     <row r="34" spans="1:1">
@@ -14197,12 +14530,12 @@
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>383</v>
+        <v>331</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>384</v>
+        <v>332</v>
       </c>
     </row>
     <row r="39" spans="1:1">
@@ -14217,12 +14550,12 @@
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>385</v>
+        <v>333</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>386</v>
+        <v>334</v>
       </c>
     </row>
     <row r="44" spans="1:1">
@@ -14237,12 +14570,12 @@
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>387</v>
+        <v>335</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>388</v>
+        <v>336</v>
       </c>
     </row>
     <row r="49" spans="1:1">
@@ -14257,12 +14590,12 @@
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="s">
-        <v>389</v>
+        <v>337</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>390</v>
+        <v>338</v>
       </c>
     </row>
     <row r="54" spans="1:1">
@@ -14282,12 +14615,12 @@
     </row>
     <row r="57" spans="1:1">
       <c r="A57" t="s">
-        <v>491</v>
+        <v>435</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" t="s">
-        <v>492</v>
+        <v>436</v>
       </c>
     </row>
     <row r="59" spans="1:1">
@@ -14307,12 +14640,12 @@
     </row>
     <row r="62" spans="1:1">
       <c r="A62" t="s">
-        <v>493</v>
+        <v>437</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" t="s">
-        <v>494</v>
+        <v>438</v>
       </c>
     </row>
     <row r="64" spans="1:1">
@@ -14332,12 +14665,12 @@
     </row>
     <row r="67" spans="1:1">
       <c r="A67" t="s">
-        <v>495</v>
+        <v>439</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" t="s">
-        <v>496</v>
+        <v>440</v>
       </c>
     </row>
     <row r="69" spans="1:1">
@@ -14357,12 +14690,12 @@
     </row>
     <row r="72" spans="1:1">
       <c r="A72" t="s">
-        <v>391</v>
+        <v>339</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" t="s">
-        <v>392</v>
+        <v>340</v>
       </c>
     </row>
     <row r="74" spans="1:1">
@@ -14377,12 +14710,12 @@
     </row>
     <row r="77" spans="1:1">
       <c r="A77" t="s">
-        <v>393</v>
+        <v>341</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" t="s">
-        <v>394</v>
+        <v>342</v>
       </c>
     </row>
     <row r="79" spans="1:1">
@@ -14397,12 +14730,12 @@
     </row>
     <row r="82" spans="1:1">
       <c r="A82" t="s">
-        <v>395</v>
+        <v>343</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" t="s">
-        <v>396</v>
+        <v>344</v>
       </c>
     </row>
     <row r="84" spans="1:1">
@@ -14417,12 +14750,12 @@
     </row>
     <row r="87" spans="1:1">
       <c r="A87" t="s">
-        <v>397</v>
+        <v>345</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" t="s">
-        <v>398</v>
+        <v>346</v>
       </c>
     </row>
     <row r="89" spans="1:1">
@@ -14442,12 +14775,12 @@
     </row>
     <row r="92" spans="1:1">
       <c r="A92" t="s">
-        <v>497</v>
+        <v>441</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" t="s">
-        <v>498</v>
+        <v>442</v>
       </c>
     </row>
     <row r="94" spans="1:1">
@@ -14462,12 +14795,12 @@
     </row>
     <row r="97" spans="1:1">
       <c r="A97" t="s">
-        <v>499</v>
+        <v>443</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" t="s">
-        <v>500</v>
+        <v>444</v>
       </c>
     </row>
     <row r="99" spans="1:1">
@@ -14482,12 +14815,12 @@
     </row>
     <row r="102" spans="1:1">
       <c r="A102" t="s">
-        <v>501</v>
+        <v>445</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" t="s">
-        <v>502</v>
+        <v>446</v>
       </c>
     </row>
     <row r="104" spans="1:1">
@@ -14507,12 +14840,12 @@
     </row>
     <row r="107" spans="1:1">
       <c r="A107" t="s">
-        <v>399</v>
+        <v>347</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108" t="s">
-        <v>400</v>
+        <v>348</v>
       </c>
     </row>
     <row r="109" spans="1:1">
@@ -14527,12 +14860,12 @@
     </row>
     <row r="112" spans="1:1">
       <c r="A112" t="s">
-        <v>401</v>
+        <v>349</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" t="s">
-        <v>402</v>
+        <v>350</v>
       </c>
     </row>
     <row r="114" spans="1:1">
@@ -14547,12 +14880,12 @@
     </row>
     <row r="117" spans="1:1">
       <c r="A117" t="s">
-        <v>403</v>
+        <v>351</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" t="s">
-        <v>404</v>
+        <v>352</v>
       </c>
     </row>
     <row r="119" spans="1:1">
@@ -14567,12 +14900,12 @@
     </row>
     <row r="122" spans="1:1">
       <c r="A122" t="s">
-        <v>405</v>
+        <v>353</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" t="s">
-        <v>406</v>
+        <v>354</v>
       </c>
     </row>
     <row r="124" spans="1:1">
@@ -14592,12 +14925,12 @@
     </row>
     <row r="127" spans="1:1">
       <c r="A127" t="s">
-        <v>503</v>
+        <v>447</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128" t="s">
-        <v>504</v>
+        <v>448</v>
       </c>
     </row>
     <row r="129" spans="1:1">
@@ -14612,12 +14945,12 @@
     </row>
     <row r="132" spans="1:1">
       <c r="A132" t="s">
-        <v>505</v>
+        <v>449</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133" t="s">
-        <v>506</v>
+        <v>450</v>
       </c>
     </row>
     <row r="134" spans="1:1">
@@ -14632,12 +14965,12 @@
     </row>
     <row r="137" spans="1:1">
       <c r="A137" t="s">
-        <v>507</v>
+        <v>451</v>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138" t="s">
-        <v>508</v>
+        <v>452</v>
       </c>
     </row>
     <row r="139" spans="1:1">
@@ -14657,12 +14990,12 @@
     </row>
     <row r="142" spans="1:1">
       <c r="A142" t="s">
-        <v>407</v>
+        <v>355</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143" t="s">
-        <v>408</v>
+        <v>356</v>
       </c>
     </row>
     <row r="144" spans="1:1">
@@ -14677,12 +15010,12 @@
     </row>
     <row r="147" spans="1:1">
       <c r="A147" t="s">
-        <v>409</v>
+        <v>357</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148" t="s">
-        <v>410</v>
+        <v>358</v>
       </c>
     </row>
     <row r="149" spans="1:1">
@@ -14697,12 +15030,12 @@
     </row>
     <row r="152" spans="1:1">
       <c r="A152" t="s">
-        <v>411</v>
+        <v>359</v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153" t="s">
-        <v>412</v>
+        <v>360</v>
       </c>
     </row>
     <row r="154" spans="1:1">
@@ -14717,12 +15050,12 @@
     </row>
     <row r="157" spans="1:1">
       <c r="A157" t="s">
-        <v>413</v>
+        <v>361</v>
       </c>
     </row>
     <row r="158" spans="1:1">
       <c r="A158" t="s">
-        <v>414</v>
+        <v>362</v>
       </c>
     </row>
     <row r="159" spans="1:1">
@@ -14737,12 +15070,12 @@
     </row>
     <row r="162" spans="1:1">
       <c r="A162" t="s">
-        <v>415</v>
+        <v>363</v>
       </c>
     </row>
     <row r="163" spans="1:1">
       <c r="A163" t="s">
-        <v>416</v>
+        <v>364</v>
       </c>
     </row>
     <row r="164" spans="1:1">
@@ -14757,12 +15090,12 @@
     </row>
     <row r="167" spans="1:1">
       <c r="A167" t="s">
-        <v>417</v>
+        <v>365</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168" t="s">
-        <v>418</v>
+        <v>366</v>
       </c>
     </row>
     <row r="169" spans="1:1">
@@ -14777,12 +15110,12 @@
     </row>
     <row r="172" spans="1:1">
       <c r="A172" t="s">
-        <v>419</v>
+        <v>367</v>
       </c>
     </row>
     <row r="173" spans="1:1">
       <c r="A173" t="s">
-        <v>420</v>
+        <v>368</v>
       </c>
     </row>
     <row r="174" spans="1:1">
@@ -14797,12 +15130,12 @@
     </row>
     <row r="177" spans="1:1">
       <c r="A177" t="s">
-        <v>421</v>
+        <v>369</v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178" t="s">
-        <v>422</v>
+        <v>370</v>
       </c>
     </row>
     <row r="179" spans="1:1">
@@ -14817,12 +15150,12 @@
     </row>
     <row r="182" spans="1:1">
       <c r="A182" t="s">
-        <v>423</v>
+        <v>371</v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183" t="s">
-        <v>424</v>
+        <v>372</v>
       </c>
     </row>
     <row r="184" spans="1:1">
@@ -14837,12 +15170,12 @@
     </row>
     <row r="187" spans="1:1">
       <c r="A187" t="s">
-        <v>425</v>
+        <v>373</v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188" t="s">
-        <v>426</v>
+        <v>374</v>
       </c>
     </row>
     <row r="189" spans="1:1">
@@ -14862,12 +15195,12 @@
     </row>
     <row r="192" spans="1:1">
       <c r="A192" t="s">
-        <v>509</v>
+        <v>453</v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193" t="s">
-        <v>510</v>
+        <v>454</v>
       </c>
     </row>
     <row r="194" spans="1:1">
@@ -14882,12 +15215,12 @@
     </row>
     <row r="197" spans="1:1">
       <c r="A197" t="s">
-        <v>511</v>
+        <v>455</v>
       </c>
     </row>
     <row r="198" spans="1:1">
       <c r="A198" t="s">
-        <v>512</v>
+        <v>456</v>
       </c>
     </row>
     <row r="199" spans="1:1">
@@ -14902,12 +15235,12 @@
     </row>
     <row r="202" spans="1:1">
       <c r="A202" t="s">
-        <v>513</v>
+        <v>457</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203" t="s">
-        <v>514</v>
+        <v>458</v>
       </c>
     </row>
     <row r="204" spans="1:1">
@@ -14922,12 +15255,12 @@
     </row>
     <row r="207" spans="1:1">
       <c r="A207" t="s">
-        <v>515</v>
+        <v>459</v>
       </c>
     </row>
     <row r="208" spans="1:1">
       <c r="A208" t="s">
-        <v>516</v>
+        <v>460</v>
       </c>
     </row>
     <row r="209" spans="1:1">
@@ -14942,12 +15275,12 @@
     </row>
     <row r="212" spans="1:1">
       <c r="A212" t="s">
-        <v>517</v>
+        <v>461</v>
       </c>
     </row>
     <row r="213" spans="1:1">
       <c r="A213" t="s">
-        <v>518</v>
+        <v>462</v>
       </c>
     </row>
     <row r="214" spans="1:1">
@@ -14962,12 +15295,12 @@
     </row>
     <row r="217" spans="1:1">
       <c r="A217" t="s">
-        <v>519</v>
+        <v>463</v>
       </c>
     </row>
     <row r="218" spans="1:1">
       <c r="A218" t="s">
-        <v>520</v>
+        <v>464</v>
       </c>
     </row>
     <row r="219" spans="1:1">
@@ -14982,12 +15315,12 @@
     </row>
     <row r="222" spans="1:1">
       <c r="A222" t="s">
-        <v>521</v>
+        <v>465</v>
       </c>
     </row>
     <row r="223" spans="1:1">
       <c r="A223" t="s">
-        <v>522</v>
+        <v>466</v>
       </c>
     </row>
     <row r="224" spans="1:1">
@@ -15002,12 +15335,12 @@
     </row>
     <row r="227" spans="1:1">
       <c r="A227" t="s">
-        <v>523</v>
+        <v>467</v>
       </c>
     </row>
     <row r="228" spans="1:1">
       <c r="A228" t="s">
-        <v>524</v>
+        <v>468</v>
       </c>
     </row>
     <row r="229" spans="1:1">
@@ -15027,12 +15360,12 @@
     </row>
     <row r="232" spans="1:1">
       <c r="A232" t="s">
-        <v>525</v>
+        <v>469</v>
       </c>
     </row>
     <row r="233" spans="1:1">
       <c r="A233" t="s">
-        <v>526</v>
+        <v>470</v>
       </c>
     </row>
     <row r="234" spans="1:1">
@@ -15052,12 +15385,12 @@
     </row>
     <row r="237" spans="1:1">
       <c r="A237" t="s">
-        <v>527</v>
+        <v>471</v>
       </c>
     </row>
     <row r="238" spans="1:1">
       <c r="A238" t="s">
-        <v>528</v>
+        <v>472</v>
       </c>
     </row>
     <row r="239" spans="1:1">
@@ -15077,12 +15410,12 @@
     </row>
     <row r="242" spans="1:1">
       <c r="A242" t="s">
-        <v>529</v>
+        <v>473</v>
       </c>
     </row>
     <row r="243" spans="1:1">
       <c r="A243" t="s">
-        <v>530</v>
+        <v>474</v>
       </c>
     </row>
     <row r="244" spans="1:1">
@@ -15102,12 +15435,12 @@
     </row>
     <row r="247" spans="1:1">
       <c r="A247" t="s">
-        <v>531</v>
+        <v>475</v>
       </c>
     </row>
     <row r="248" spans="1:1">
       <c r="A248" t="s">
-        <v>532</v>
+        <v>476</v>
       </c>
     </row>
     <row r="249" spans="1:1">
@@ -15127,12 +15460,12 @@
     </row>
     <row r="252" spans="1:1">
       <c r="A252" t="s">
-        <v>533</v>
+        <v>477</v>
       </c>
     </row>
     <row r="253" spans="1:1">
       <c r="A253" t="s">
-        <v>534</v>
+        <v>478</v>
       </c>
     </row>
     <row r="254" spans="1:1">
@@ -15152,12 +15485,12 @@
     </row>
     <row r="257" spans="1:1">
       <c r="A257" t="s">
-        <v>535</v>
+        <v>479</v>
       </c>
     </row>
     <row r="258" spans="1:1">
       <c r="A258" t="s">
-        <v>536</v>
+        <v>480</v>
       </c>
     </row>
     <row r="259" spans="1:1">
@@ -15177,12 +15510,12 @@
     </row>
     <row r="262" spans="1:1">
       <c r="A262" t="s">
-        <v>537</v>
+        <v>481</v>
       </c>
     </row>
     <row r="263" spans="1:1">
       <c r="A263" t="s">
-        <v>538</v>
+        <v>482</v>
       </c>
     </row>
     <row r="264" spans="1:1">
@@ -15202,12 +15535,12 @@
     </row>
     <row r="267" spans="1:1">
       <c r="A267" t="s">
-        <v>539</v>
+        <v>483</v>
       </c>
     </row>
     <row r="268" spans="1:1">
       <c r="A268" t="s">
-        <v>540</v>
+        <v>484</v>
       </c>
     </row>
     <row r="269" spans="1:1">
@@ -15224,4 +15557,1224 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A269"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1">
+      <c r="A122" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1">
+      <c r="A123" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1">
+      <c r="A124" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1">
+      <c r="A125" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1">
+      <c r="A126" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1">
+      <c r="A127" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1">
+      <c r="A128" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1">
+      <c r="A129" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1">
+      <c r="A132" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1">
+      <c r="A133" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1">
+      <c r="A134" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1">
+      <c r="A136" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1">
+      <c r="A137" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1">
+      <c r="A138" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1">
+      <c r="A139" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1">
+      <c r="A140" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1">
+      <c r="A141" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1">
+      <c r="A142" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1">
+      <c r="A143" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1">
+      <c r="A144" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1">
+      <c r="A146" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1">
+      <c r="A147" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1">
+      <c r="A148" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1">
+      <c r="A149" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1">
+      <c r="A151" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1">
+      <c r="A152" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1">
+      <c r="A153" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1">
+      <c r="A154" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1">
+      <c r="A156" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1">
+      <c r="A157" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1">
+      <c r="A158" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1">
+      <c r="A159" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1">
+      <c r="A161" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1">
+      <c r="A162" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1">
+      <c r="A163" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1">
+      <c r="A164" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1">
+      <c r="A166" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1">
+      <c r="A167" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1">
+      <c r="A168" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1">
+      <c r="A169" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1">
+      <c r="A171" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1">
+      <c r="A172" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1">
+      <c r="A173" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1">
+      <c r="A174" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1">
+      <c r="A176" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1">
+      <c r="A177" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1">
+      <c r="A178" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1">
+      <c r="A179" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1">
+      <c r="A181" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1">
+      <c r="A182" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1">
+      <c r="A183" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1">
+      <c r="A184" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1">
+      <c r="A186" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1">
+      <c r="A187" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1">
+      <c r="A188" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1">
+      <c r="A189" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1">
+      <c r="A190" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1">
+      <c r="A191" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1">
+      <c r="A192" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1">
+      <c r="A193" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1">
+      <c r="A194" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1">
+      <c r="A196" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1">
+      <c r="A197" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1">
+      <c r="A198" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1">
+      <c r="A199" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1">
+      <c r="A201" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1">
+      <c r="A202" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1">
+      <c r="A203" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1">
+      <c r="A204" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1">
+      <c r="A206" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1">
+      <c r="A207" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1">
+      <c r="A208" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1">
+      <c r="A209" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1">
+      <c r="A211" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1">
+      <c r="A212" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1">
+      <c r="A213" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1">
+      <c r="A214" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1">
+      <c r="A216" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1">
+      <c r="A217" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1">
+      <c r="A218" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1">
+      <c r="A219" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1">
+      <c r="A221" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1">
+      <c r="A222" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1">
+      <c r="A223" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1">
+      <c r="A224" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1">
+      <c r="A226" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1">
+      <c r="A227" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1">
+      <c r="A228" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1">
+      <c r="A229" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1">
+      <c r="A230" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1">
+      <c r="A231" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1">
+      <c r="A232" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1">
+      <c r="A233" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1">
+      <c r="A234" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1">
+      <c r="A235" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1">
+      <c r="A236" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1">
+      <c r="A237" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1">
+      <c r="A238" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1">
+      <c r="A239" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1">
+      <c r="A240" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1">
+      <c r="A241" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1">
+      <c r="A242" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1">
+      <c r="A243" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1">
+      <c r="A244" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1">
+      <c r="A245" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1">
+      <c r="A246" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1">
+      <c r="A247" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1">
+      <c r="A248" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1">
+      <c r="A249" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1">
+      <c r="A250" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1">
+      <c r="A251" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1">
+      <c r="A252" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1">
+      <c r="A253" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1">
+      <c r="A254" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1">
+      <c r="A255" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1">
+      <c r="A256" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1">
+      <c r="A257" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1">
+      <c r="A258" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1">
+      <c r="A259" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1">
+      <c r="A260" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1">
+      <c r="A261" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1">
+      <c r="A262" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1">
+      <c r="A263" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1">
+      <c r="A264" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1">
+      <c r="A265" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1">
+      <c r="A266" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1">
+      <c r="A267" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1">
+      <c r="A268" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1">
+      <c r="A269" t="s">
+        <v>319</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>